<commit_message>
minor edits trying to get this running on another machine
</commit_message>
<xml_diff>
--- a/data/2021.xlsx
+++ b/data/2021.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="23901"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="24729"/>
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\R_Projects\riverLottery\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{13BB1683-1670-4FCF-AF89-82D42C9E565C}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DFF8B816-A673-4701-B2B3-E943139BA0E0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" tabRatio="652" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-98" yWindow="-98" windowWidth="20715" windowHeight="13276" tabRatio="652" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="2021 Middle Fork Salmon" sheetId="6" r:id="rId1"/>
@@ -36,41 +36,6 @@
     </ext>
   </extLst>
 </workbook>
-</file>
-
-<file path=xl/comments1.xml><?xml version="1.0" encoding="utf-8"?>
-<comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr">
-  <authors>
-    <author>Donna Leuzinger</author>
-  </authors>
-  <commentList>
-    <comment ref="A64" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0200-000002000000}">
-      <text>
-        <r>
-          <rPr>
-            <b/>
-            <sz val="9"/>
-            <color indexed="81"/>
-            <rFont val="Tahoma"/>
-            <family val="2"/>
-          </rPr>
-          <t>Donna Leuzinger:</t>
-        </r>
-        <r>
-          <rPr>
-            <sz val="9"/>
-            <color indexed="81"/>
-            <rFont val="Tahoma"/>
-            <family val="2"/>
-          </rPr>
-          <t xml:space="preserve">
-Edit Year in Sheet Names to update year in Header.
-</t>
-        </r>
-      </text>
-    </comment>
-  </commentList>
-</comments>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
@@ -120,7 +85,7 @@
     <numFmt numFmtId="43" formatCode="_(* #,##0.00_);_(* \(#,##0.00\);_(* &quot;-&quot;??_);_(@_)"/>
     <numFmt numFmtId="164" formatCode="_(* #,##0_);_(* \(#,##0\);_(* &quot;-&quot;??_);_(@_)"/>
   </numFmts>
-  <fonts count="8" x14ac:knownFonts="1">
+  <fonts count="6" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -148,19 +113,6 @@
       <sz val="10"/>
       <color theme="1"/>
       <name val="Arial"/>
-      <family val="2"/>
-    </font>
-    <font>
-      <sz val="9"/>
-      <color indexed="81"/>
-      <name val="Tahoma"/>
-      <family val="2"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="9"/>
-      <color indexed="81"/>
-      <name val="Tahoma"/>
       <family val="2"/>
     </font>
     <font>
@@ -216,7 +168,7 @@
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0"/>
     <xf numFmtId="43" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="43" fontId="7" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="43" fontId="5" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
   <cellXfs count="19">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
@@ -826,19 +778,19 @@
       <selection pane="bottomLeft" activeCell="I1" sqref="I1:I1048576"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9" defaultRowHeight="13.2" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="9" defaultRowHeight="13.15" x14ac:dyDescent="0.4"/>
   <cols>
-    <col min="1" max="1" width="14.09765625" style="11" customWidth="1"/>
-    <col min="2" max="2" width="9.59765625" style="12" customWidth="1"/>
+    <col min="1" max="1" width="14.125" style="11" customWidth="1"/>
+    <col min="2" max="2" width="9.625" style="12" customWidth="1"/>
     <col min="3" max="3" width="9" style="12" customWidth="1"/>
-    <col min="4" max="5" width="8.59765625" style="12" customWidth="1"/>
-    <col min="6" max="6" width="9.59765625" style="10" customWidth="1"/>
-    <col min="7" max="7" width="3.59765625" style="7" customWidth="1"/>
-    <col min="8" max="8" width="31.09765625" style="12" customWidth="1"/>
+    <col min="4" max="5" width="8.625" style="12" customWidth="1"/>
+    <col min="6" max="6" width="9.625" style="10" customWidth="1"/>
+    <col min="7" max="7" width="3.625" style="7" customWidth="1"/>
+    <col min="8" max="8" width="31.125" style="12" customWidth="1"/>
     <col min="9" max="16384" width="9" style="7"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" ht="52.8" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:8" ht="52.5" x14ac:dyDescent="0.4">
       <c r="A1" s="1" t="s">
         <v>8</v>
       </c>
@@ -862,7 +814,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="2" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:8" x14ac:dyDescent="0.4">
       <c r="A2" s="4">
         <v>44344</v>
       </c>
@@ -886,7 +838,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="3" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:8" x14ac:dyDescent="0.4">
       <c r="A3" s="4">
         <v>44345</v>
       </c>
@@ -910,7 +862,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="4" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:8" x14ac:dyDescent="0.4">
       <c r="A4" s="4">
         <v>44346</v>
       </c>
@@ -934,7 +886,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="5" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:8" x14ac:dyDescent="0.4">
       <c r="A5" s="4">
         <v>44347</v>
       </c>
@@ -958,7 +910,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="6" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:8" x14ac:dyDescent="0.4">
       <c r="A6" s="4">
         <v>44348</v>
       </c>
@@ -982,7 +934,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="7" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:8" x14ac:dyDescent="0.4">
       <c r="A7" s="4">
         <v>44349</v>
       </c>
@@ -1006,7 +958,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="8" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:8" x14ac:dyDescent="0.4">
       <c r="A8" s="4">
         <v>44350</v>
       </c>
@@ -1030,7 +982,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="9" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:8" x14ac:dyDescent="0.4">
       <c r="A9" s="4">
         <v>44351</v>
       </c>
@@ -1054,7 +1006,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="10" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:8" x14ac:dyDescent="0.4">
       <c r="A10" s="4">
         <v>44352</v>
       </c>
@@ -1078,7 +1030,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="11" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:8" x14ac:dyDescent="0.4">
       <c r="A11" s="4">
         <v>44353</v>
       </c>
@@ -1102,7 +1054,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="12" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:8" x14ac:dyDescent="0.4">
       <c r="A12" s="4">
         <v>44354</v>
       </c>
@@ -1126,7 +1078,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="13" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:8" x14ac:dyDescent="0.4">
       <c r="A13" s="4">
         <v>44355</v>
       </c>
@@ -1150,7 +1102,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="14" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:8" x14ac:dyDescent="0.4">
       <c r="A14" s="4">
         <v>44356</v>
       </c>
@@ -1174,7 +1126,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="15" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:8" x14ac:dyDescent="0.4">
       <c r="A15" s="4">
         <v>44357</v>
       </c>
@@ -1198,7 +1150,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="16" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:8" x14ac:dyDescent="0.4">
       <c r="A16" s="4">
         <v>44358</v>
       </c>
@@ -1222,7 +1174,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="17" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:8" x14ac:dyDescent="0.4">
       <c r="A17" s="4">
         <v>44359</v>
       </c>
@@ -1246,7 +1198,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="18" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:8" x14ac:dyDescent="0.4">
       <c r="A18" s="4">
         <v>44360</v>
       </c>
@@ -1270,7 +1222,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="19" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:8" x14ac:dyDescent="0.4">
       <c r="A19" s="4">
         <v>44361</v>
       </c>
@@ -1294,7 +1246,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="20" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:8" x14ac:dyDescent="0.4">
       <c r="A20" s="4">
         <v>44362</v>
       </c>
@@ -1318,7 +1270,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="21" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:8" x14ac:dyDescent="0.4">
       <c r="A21" s="4">
         <v>44363</v>
       </c>
@@ -1342,7 +1294,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="22" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:8" x14ac:dyDescent="0.4">
       <c r="A22" s="4">
         <v>44364</v>
       </c>
@@ -1366,7 +1318,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="23" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:8" x14ac:dyDescent="0.4">
       <c r="A23" s="4">
         <v>44365</v>
       </c>
@@ -1390,7 +1342,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="24" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:8" x14ac:dyDescent="0.4">
       <c r="A24" s="4">
         <v>44366</v>
       </c>
@@ -1414,7 +1366,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="25" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:8" x14ac:dyDescent="0.4">
       <c r="A25" s="4">
         <v>44367</v>
       </c>
@@ -1438,7 +1390,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="26" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:8" x14ac:dyDescent="0.4">
       <c r="A26" s="4">
         <v>44368</v>
       </c>
@@ -1462,7 +1414,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="27" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:8" x14ac:dyDescent="0.4">
       <c r="A27" s="4">
         <v>44369</v>
       </c>
@@ -1486,7 +1438,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="28" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:8" x14ac:dyDescent="0.4">
       <c r="A28" s="4">
         <v>44370</v>
       </c>
@@ -1510,7 +1462,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="29" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:8" x14ac:dyDescent="0.4">
       <c r="A29" s="4">
         <v>44371</v>
       </c>
@@ -1534,7 +1486,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="30" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:8" x14ac:dyDescent="0.4">
       <c r="A30" s="4">
         <v>44372</v>
       </c>
@@ -1558,7 +1510,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="31" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:8" x14ac:dyDescent="0.4">
       <c r="A31" s="4">
         <v>44373</v>
       </c>
@@ -1582,7 +1534,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="32" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:8" x14ac:dyDescent="0.4">
       <c r="A32" s="4">
         <v>44374</v>
       </c>
@@ -1606,7 +1558,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="33" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:8" x14ac:dyDescent="0.4">
       <c r="A33" s="4">
         <v>44375</v>
       </c>
@@ -1630,7 +1582,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="34" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:8" x14ac:dyDescent="0.4">
       <c r="A34" s="4">
         <v>44376</v>
       </c>
@@ -1654,7 +1606,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="35" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:8" x14ac:dyDescent="0.4">
       <c r="A35" s="4">
         <v>44377</v>
       </c>
@@ -1678,7 +1630,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="36" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:8" x14ac:dyDescent="0.4">
       <c r="A36" s="4">
         <v>44378</v>
       </c>
@@ -1702,7 +1654,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="37" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:8" x14ac:dyDescent="0.4">
       <c r="A37" s="4">
         <v>44379</v>
       </c>
@@ -1726,7 +1678,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="38" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:8" x14ac:dyDescent="0.4">
       <c r="A38" s="4">
         <v>44380</v>
       </c>
@@ -1750,7 +1702,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="39" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:8" x14ac:dyDescent="0.4">
       <c r="A39" s="4">
         <v>44381</v>
       </c>
@@ -1774,7 +1726,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="40" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:8" x14ac:dyDescent="0.4">
       <c r="A40" s="4">
         <v>44382</v>
       </c>
@@ -1798,7 +1750,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="41" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:8" x14ac:dyDescent="0.4">
       <c r="A41" s="4">
         <v>44383</v>
       </c>
@@ -1822,7 +1774,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="42" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:8" x14ac:dyDescent="0.4">
       <c r="A42" s="4">
         <v>44384</v>
       </c>
@@ -1846,7 +1798,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="43" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="43" spans="1:8" x14ac:dyDescent="0.4">
       <c r="A43" s="4">
         <v>44385</v>
       </c>
@@ -1870,7 +1822,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="44" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="44" spans="1:8" x14ac:dyDescent="0.4">
       <c r="A44" s="4">
         <v>44386</v>
       </c>
@@ -1894,7 +1846,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="45" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="45" spans="1:8" x14ac:dyDescent="0.4">
       <c r="A45" s="4">
         <v>44387</v>
       </c>
@@ -1918,7 +1870,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="46" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="46" spans="1:8" x14ac:dyDescent="0.4">
       <c r="A46" s="4">
         <v>44388</v>
       </c>
@@ -1942,7 +1894,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="47" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="47" spans="1:8" x14ac:dyDescent="0.4">
       <c r="A47" s="4">
         <v>44389</v>
       </c>
@@ -1966,7 +1918,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="48" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="48" spans="1:8" x14ac:dyDescent="0.4">
       <c r="A48" s="4">
         <v>44390</v>
       </c>
@@ -1990,7 +1942,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="49" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="49" spans="1:8" x14ac:dyDescent="0.4">
       <c r="A49" s="4">
         <v>44391</v>
       </c>
@@ -2014,7 +1966,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="50" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="50" spans="1:8" x14ac:dyDescent="0.4">
       <c r="A50" s="4">
         <v>44392</v>
       </c>
@@ -2038,7 +1990,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="51" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="51" spans="1:8" x14ac:dyDescent="0.4">
       <c r="A51" s="4">
         <v>44393</v>
       </c>
@@ -2062,7 +2014,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="52" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="52" spans="1:8" x14ac:dyDescent="0.4">
       <c r="A52" s="4">
         <v>44394</v>
       </c>
@@ -2086,7 +2038,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="53" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="53" spans="1:8" x14ac:dyDescent="0.4">
       <c r="A53" s="4">
         <v>44395</v>
       </c>
@@ -2110,7 +2062,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="54" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="54" spans="1:8" x14ac:dyDescent="0.4">
       <c r="A54" s="4">
         <v>44396</v>
       </c>
@@ -2134,7 +2086,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="55" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="55" spans="1:8" x14ac:dyDescent="0.4">
       <c r="A55" s="4">
         <v>44397</v>
       </c>
@@ -2158,7 +2110,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="56" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="56" spans="1:8" x14ac:dyDescent="0.4">
       <c r="A56" s="4">
         <v>44398</v>
       </c>
@@ -2182,7 +2134,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="57" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="57" spans="1:8" x14ac:dyDescent="0.4">
       <c r="A57" s="4">
         <v>44399</v>
       </c>
@@ -2206,7 +2158,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="58" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="58" spans="1:8" x14ac:dyDescent="0.4">
       <c r="A58" s="4">
         <v>44400</v>
       </c>
@@ -2230,7 +2182,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="59" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="59" spans="1:8" x14ac:dyDescent="0.4">
       <c r="A59" s="4">
         <v>44401</v>
       </c>
@@ -2254,7 +2206,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="60" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="60" spans="1:8" x14ac:dyDescent="0.4">
       <c r="A60" s="4">
         <v>44402</v>
       </c>
@@ -2278,7 +2230,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="61" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="61" spans="1:8" x14ac:dyDescent="0.4">
       <c r="A61" s="4">
         <v>44403</v>
       </c>
@@ -2302,7 +2254,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="62" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="62" spans="1:8" x14ac:dyDescent="0.4">
       <c r="A62" s="4">
         <v>44404</v>
       </c>
@@ -2326,7 +2278,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="63" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="63" spans="1:8" x14ac:dyDescent="0.4">
       <c r="A63" s="4">
         <v>44405</v>
       </c>
@@ -2350,7 +2302,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="64" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="64" spans="1:8" x14ac:dyDescent="0.4">
       <c r="A64" s="4">
         <v>44406</v>
       </c>
@@ -2374,7 +2326,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="65" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="65" spans="1:8" x14ac:dyDescent="0.4">
       <c r="A65" s="4">
         <v>44407</v>
       </c>
@@ -2398,7 +2350,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="66" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="66" spans="1:8" x14ac:dyDescent="0.4">
       <c r="A66" s="4">
         <v>44408</v>
       </c>
@@ -2422,7 +2374,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="67" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="67" spans="1:8" x14ac:dyDescent="0.4">
       <c r="A67" s="4">
         <v>44409</v>
       </c>
@@ -2446,7 +2398,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="68" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="68" spans="1:8" x14ac:dyDescent="0.4">
       <c r="A68" s="4">
         <v>44410</v>
       </c>
@@ -2470,7 +2422,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="69" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="69" spans="1:8" x14ac:dyDescent="0.4">
       <c r="A69" s="4">
         <v>44411</v>
       </c>
@@ -2494,7 +2446,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="70" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="70" spans="1:8" x14ac:dyDescent="0.4">
       <c r="A70" s="4">
         <v>44412</v>
       </c>
@@ -2518,7 +2470,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="71" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="71" spans="1:8" x14ac:dyDescent="0.4">
       <c r="A71" s="4">
         <v>44413</v>
       </c>
@@ -2542,7 +2494,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="72" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="72" spans="1:8" x14ac:dyDescent="0.4">
       <c r="A72" s="4">
         <v>44414</v>
       </c>
@@ -2566,7 +2518,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="73" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="73" spans="1:8" x14ac:dyDescent="0.4">
       <c r="A73" s="4">
         <v>44415</v>
       </c>
@@ -2590,7 +2542,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="74" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="74" spans="1:8" x14ac:dyDescent="0.4">
       <c r="A74" s="4">
         <v>44416</v>
       </c>
@@ -2614,7 +2566,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="75" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="75" spans="1:8" x14ac:dyDescent="0.4">
       <c r="A75" s="4">
         <v>44417</v>
       </c>
@@ -2638,7 +2590,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="76" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="76" spans="1:8" x14ac:dyDescent="0.4">
       <c r="A76" s="4">
         <v>44418</v>
       </c>
@@ -2662,7 +2614,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="77" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="77" spans="1:8" x14ac:dyDescent="0.4">
       <c r="A77" s="4">
         <v>44419</v>
       </c>
@@ -2686,7 +2638,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="78" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="78" spans="1:8" x14ac:dyDescent="0.4">
       <c r="A78" s="4">
         <v>44420</v>
       </c>
@@ -2710,7 +2662,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="79" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="79" spans="1:8" x14ac:dyDescent="0.4">
       <c r="A79" s="4">
         <v>44421</v>
       </c>
@@ -2734,7 +2686,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="80" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="80" spans="1:8" x14ac:dyDescent="0.4">
       <c r="A80" s="4">
         <v>44422</v>
       </c>
@@ -2758,7 +2710,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="81" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="81" spans="1:8" x14ac:dyDescent="0.4">
       <c r="A81" s="4">
         <v>44423</v>
       </c>
@@ -2782,7 +2734,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="82" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="82" spans="1:8" x14ac:dyDescent="0.4">
       <c r="A82" s="4">
         <v>44424</v>
       </c>
@@ -2806,7 +2758,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="83" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="83" spans="1:8" x14ac:dyDescent="0.4">
       <c r="A83" s="4">
         <v>44425</v>
       </c>
@@ -2830,7 +2782,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="84" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="84" spans="1:8" x14ac:dyDescent="0.4">
       <c r="A84" s="4">
         <v>44426</v>
       </c>
@@ -2854,7 +2806,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="85" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="85" spans="1:8" x14ac:dyDescent="0.4">
       <c r="A85" s="4">
         <v>44427</v>
       </c>
@@ -2878,7 +2830,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="86" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="86" spans="1:8" x14ac:dyDescent="0.4">
       <c r="A86" s="4">
         <v>44428</v>
       </c>
@@ -2902,7 +2854,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="87" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="87" spans="1:8" x14ac:dyDescent="0.4">
       <c r="A87" s="4">
         <v>44429</v>
       </c>
@@ -2926,7 +2878,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="88" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="88" spans="1:8" x14ac:dyDescent="0.4">
       <c r="A88" s="4">
         <v>44430</v>
       </c>
@@ -2950,7 +2902,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="89" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="89" spans="1:8" x14ac:dyDescent="0.4">
       <c r="A89" s="4">
         <v>44431</v>
       </c>
@@ -2974,7 +2926,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="90" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="90" spans="1:8" x14ac:dyDescent="0.4">
       <c r="A90" s="4">
         <v>44432</v>
       </c>
@@ -2998,7 +2950,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="91" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="91" spans="1:8" x14ac:dyDescent="0.4">
       <c r="A91" s="4">
         <v>44433</v>
       </c>
@@ -3022,7 +2974,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="92" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="92" spans="1:8" x14ac:dyDescent="0.4">
       <c r="A92" s="4">
         <v>44434</v>
       </c>
@@ -3046,7 +2998,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="93" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="93" spans="1:8" x14ac:dyDescent="0.4">
       <c r="A93" s="4">
         <v>44435</v>
       </c>
@@ -3070,7 +3022,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="94" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="94" spans="1:8" x14ac:dyDescent="0.4">
       <c r="A94" s="4">
         <v>44436</v>
       </c>
@@ -3094,7 +3046,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="95" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="95" spans="1:8" x14ac:dyDescent="0.4">
       <c r="A95" s="4">
         <v>44437</v>
       </c>
@@ -3118,7 +3070,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="96" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="96" spans="1:8" x14ac:dyDescent="0.4">
       <c r="A96" s="4">
         <v>44438</v>
       </c>
@@ -3142,7 +3094,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="97" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="97" spans="1:8" x14ac:dyDescent="0.4">
       <c r="A97" s="4">
         <v>44439</v>
       </c>
@@ -3166,7 +3118,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="98" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="98" spans="1:8" x14ac:dyDescent="0.4">
       <c r="A98" s="4">
         <v>44440</v>
       </c>
@@ -3190,7 +3142,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="99" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="99" spans="1:8" x14ac:dyDescent="0.4">
       <c r="A99" s="4">
         <v>44441</v>
       </c>
@@ -3214,7 +3166,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="100" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="100" spans="1:8" x14ac:dyDescent="0.4">
       <c r="A100" s="4">
         <v>44442</v>
       </c>
@@ -3238,7 +3190,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="101" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="101" spans="1:8" x14ac:dyDescent="0.4">
       <c r="A101" s="8" t="s">
         <v>5</v>
       </c>
@@ -3315,20 +3267,20 @@
       <selection pane="bottomLeft" activeCell="H1" sqref="H1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9" defaultRowHeight="13.2" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="9" defaultRowHeight="13.15" x14ac:dyDescent="0.4"/>
   <cols>
     <col min="1" max="1" width="12" style="11" customWidth="1"/>
-    <col min="2" max="2" width="9.69921875" style="12" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="9.09765625" style="12" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="8.8984375" style="12" customWidth="1"/>
-    <col min="5" max="5" width="8.59765625" style="12" customWidth="1"/>
-    <col min="6" max="6" width="9.59765625" style="10" customWidth="1"/>
-    <col min="7" max="7" width="3.59765625" style="7" customWidth="1"/>
-    <col min="8" max="8" width="8.69921875" style="12" customWidth="1"/>
+    <col min="2" max="2" width="9.6875" style="12" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="9.125" style="12" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="8.875" style="12" customWidth="1"/>
+    <col min="5" max="5" width="8.625" style="12" customWidth="1"/>
+    <col min="6" max="6" width="9.625" style="10" customWidth="1"/>
+    <col min="7" max="7" width="3.625" style="7" customWidth="1"/>
+    <col min="8" max="8" width="8.6875" style="12" customWidth="1"/>
     <col min="9" max="16384" width="9" style="7"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" s="3" customFormat="1" ht="52.8" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:8" s="3" customFormat="1" ht="52.5" x14ac:dyDescent="0.4">
       <c r="A1" s="1" t="s">
         <v>9</v>
       </c>
@@ -3351,7 +3303,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="2" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:8" ht="12.75" x14ac:dyDescent="0.35">
       <c r="A2" s="4">
         <v>44367</v>
       </c>
@@ -3375,7 +3327,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="3" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:8" ht="12.75" x14ac:dyDescent="0.35">
       <c r="A3" s="4">
         <v>44368</v>
       </c>
@@ -3399,7 +3351,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="4" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:8" ht="12.75" x14ac:dyDescent="0.35">
       <c r="A4" s="4">
         <v>44369</v>
       </c>
@@ -3423,7 +3375,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="5" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:8" ht="12.75" x14ac:dyDescent="0.35">
       <c r="A5" s="4">
         <v>44370</v>
       </c>
@@ -3447,7 +3399,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="6" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:8" ht="12.75" x14ac:dyDescent="0.35">
       <c r="A6" s="4">
         <v>44371</v>
       </c>
@@ -3471,7 +3423,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="7" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:8" ht="12.75" x14ac:dyDescent="0.35">
       <c r="A7" s="4">
         <v>44372</v>
       </c>
@@ -3495,7 +3447,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="8" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:8" ht="12.75" x14ac:dyDescent="0.35">
       <c r="A8" s="4">
         <v>44373</v>
       </c>
@@ -3519,7 +3471,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="9" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:8" ht="12.75" x14ac:dyDescent="0.35">
       <c r="A9" s="4">
         <v>44374</v>
       </c>
@@ -3543,7 +3495,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="10" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:8" ht="12.75" x14ac:dyDescent="0.35">
       <c r="A10" s="4">
         <v>44375</v>
       </c>
@@ -3567,7 +3519,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="11" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:8" ht="12.75" x14ac:dyDescent="0.35">
       <c r="A11" s="4">
         <v>44376</v>
       </c>
@@ -3591,7 +3543,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="12" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:8" ht="12.75" x14ac:dyDescent="0.35">
       <c r="A12" s="4">
         <v>44377</v>
       </c>
@@ -3615,7 +3567,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="13" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:8" ht="12.75" x14ac:dyDescent="0.35">
       <c r="A13" s="4">
         <v>44378</v>
       </c>
@@ -3639,7 +3591,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="14" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:8" ht="12.75" x14ac:dyDescent="0.35">
       <c r="A14" s="4">
         <v>44379</v>
       </c>
@@ -3663,7 +3615,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="15" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:8" ht="12.75" x14ac:dyDescent="0.35">
       <c r="A15" s="4">
         <v>44380</v>
       </c>
@@ -3687,7 +3639,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="16" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:8" ht="12.75" x14ac:dyDescent="0.35">
       <c r="A16" s="4">
         <v>44381</v>
       </c>
@@ -3711,7 +3663,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="17" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:8" ht="12.75" x14ac:dyDescent="0.35">
       <c r="A17" s="4">
         <v>44382</v>
       </c>
@@ -3735,7 +3687,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="18" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:8" ht="12.75" x14ac:dyDescent="0.35">
       <c r="A18" s="4">
         <v>44383</v>
       </c>
@@ -3759,7 +3711,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="19" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:8" ht="12.75" x14ac:dyDescent="0.35">
       <c r="A19" s="4">
         <v>44384</v>
       </c>
@@ -3783,7 +3735,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="20" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:8" ht="12.75" x14ac:dyDescent="0.35">
       <c r="A20" s="4">
         <v>44385</v>
       </c>
@@ -3807,7 +3759,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="21" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:8" ht="12.75" x14ac:dyDescent="0.35">
       <c r="A21" s="4">
         <v>44386</v>
       </c>
@@ -3831,7 +3783,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="22" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:8" ht="12.75" x14ac:dyDescent="0.35">
       <c r="A22" s="4">
         <v>44387</v>
       </c>
@@ -3855,7 +3807,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="23" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:8" ht="12.75" x14ac:dyDescent="0.35">
       <c r="A23" s="4">
         <v>44388</v>
       </c>
@@ -3879,7 +3831,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="24" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:8" ht="12.75" x14ac:dyDescent="0.35">
       <c r="A24" s="4">
         <v>44389</v>
       </c>
@@ -3903,7 +3855,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="25" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:8" ht="12.75" x14ac:dyDescent="0.35">
       <c r="A25" s="4">
         <v>44390</v>
       </c>
@@ -3927,7 +3879,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="26" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:8" ht="12.75" x14ac:dyDescent="0.35">
       <c r="A26" s="4">
         <v>44391</v>
       </c>
@@ -3951,7 +3903,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="27" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:8" ht="12.75" x14ac:dyDescent="0.35">
       <c r="A27" s="4">
         <v>44392</v>
       </c>
@@ -3975,7 +3927,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="28" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:8" ht="12.75" x14ac:dyDescent="0.35">
       <c r="A28" s="4">
         <v>44393</v>
       </c>
@@ -3999,7 +3951,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="29" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:8" ht="12.75" x14ac:dyDescent="0.35">
       <c r="A29" s="4">
         <v>44394</v>
       </c>
@@ -4023,7 +3975,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="30" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:8" ht="12.75" x14ac:dyDescent="0.35">
       <c r="A30" s="4">
         <v>44395</v>
       </c>
@@ -4047,7 +3999,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="31" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:8" ht="12.75" x14ac:dyDescent="0.35">
       <c r="A31" s="4">
         <v>44396</v>
       </c>
@@ -4071,7 +4023,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="32" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:8" ht="12.75" x14ac:dyDescent="0.35">
       <c r="A32" s="4">
         <v>44397</v>
       </c>
@@ -4095,7 +4047,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="33" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:8" ht="12.75" x14ac:dyDescent="0.35">
       <c r="A33" s="4">
         <v>44398</v>
       </c>
@@ -4119,7 +4071,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="34" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:8" ht="12.75" x14ac:dyDescent="0.35">
       <c r="A34" s="4">
         <v>44399</v>
       </c>
@@ -4143,7 +4095,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="35" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:8" ht="12.75" x14ac:dyDescent="0.35">
       <c r="A35" s="4">
         <v>44400</v>
       </c>
@@ -4167,7 +4119,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="36" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:8" ht="12.75" x14ac:dyDescent="0.35">
       <c r="A36" s="4">
         <v>44401</v>
       </c>
@@ -4191,7 +4143,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="37" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:8" ht="12.75" x14ac:dyDescent="0.35">
       <c r="A37" s="4">
         <v>44402</v>
       </c>
@@ -4215,7 +4167,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="38" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:8" ht="12.75" x14ac:dyDescent="0.35">
       <c r="A38" s="4">
         <v>44403</v>
       </c>
@@ -4239,7 +4191,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="39" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:8" ht="12.75" x14ac:dyDescent="0.35">
       <c r="A39" s="4">
         <v>44404</v>
       </c>
@@ -4263,7 +4215,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="40" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:8" ht="12.75" x14ac:dyDescent="0.35">
       <c r="A40" s="4">
         <v>44405</v>
       </c>
@@ -4287,7 +4239,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="41" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:8" ht="12.75" x14ac:dyDescent="0.35">
       <c r="A41" s="4">
         <v>44406</v>
       </c>
@@ -4311,7 +4263,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="42" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:8" ht="12.75" x14ac:dyDescent="0.35">
       <c r="A42" s="4">
         <v>44407</v>
       </c>
@@ -4335,7 +4287,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="43" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="43" spans="1:8" ht="12.75" x14ac:dyDescent="0.35">
       <c r="A43" s="4">
         <v>44408</v>
       </c>
@@ -4359,7 +4311,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="44" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="44" spans="1:8" ht="12.75" x14ac:dyDescent="0.35">
       <c r="A44" s="4">
         <v>44409</v>
       </c>
@@ -4383,7 +4335,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="45" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="45" spans="1:8" ht="12.75" x14ac:dyDescent="0.35">
       <c r="A45" s="4">
         <v>44410</v>
       </c>
@@ -4407,7 +4359,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="46" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="46" spans="1:8" ht="12.75" x14ac:dyDescent="0.35">
       <c r="A46" s="4">
         <v>44411</v>
       </c>
@@ -4431,7 +4383,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="47" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="47" spans="1:8" ht="12.75" x14ac:dyDescent="0.35">
       <c r="A47" s="4">
         <v>44412</v>
       </c>
@@ -4455,7 +4407,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="48" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="48" spans="1:8" ht="12.75" x14ac:dyDescent="0.35">
       <c r="A48" s="4">
         <v>44413</v>
       </c>
@@ -4479,7 +4431,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="49" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="49" spans="1:8" ht="12.75" x14ac:dyDescent="0.35">
       <c r="A49" s="4">
         <v>44414</v>
       </c>
@@ -4503,7 +4455,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="50" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="50" spans="1:8" ht="12.75" x14ac:dyDescent="0.35">
       <c r="A50" s="4">
         <v>44415</v>
       </c>
@@ -4527,7 +4479,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="51" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="51" spans="1:8" ht="12.75" x14ac:dyDescent="0.35">
       <c r="A51" s="4">
         <v>44416</v>
       </c>
@@ -4551,7 +4503,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="52" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="52" spans="1:8" ht="12.75" x14ac:dyDescent="0.35">
       <c r="A52" s="4">
         <v>44417</v>
       </c>
@@ -4575,7 +4527,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="53" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="53" spans="1:8" ht="12.75" x14ac:dyDescent="0.35">
       <c r="A53" s="4">
         <v>44418</v>
       </c>
@@ -4599,7 +4551,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="54" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="54" spans="1:8" ht="12.75" x14ac:dyDescent="0.35">
       <c r="A54" s="4">
         <v>44419</v>
       </c>
@@ -4623,7 +4575,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="55" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="55" spans="1:8" ht="12.75" x14ac:dyDescent="0.35">
       <c r="A55" s="4">
         <v>44420</v>
       </c>
@@ -4647,7 +4599,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="56" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="56" spans="1:8" ht="12.75" x14ac:dyDescent="0.35">
       <c r="A56" s="4">
         <v>44421</v>
       </c>
@@ -4671,7 +4623,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="57" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="57" spans="1:8" ht="12.75" x14ac:dyDescent="0.35">
       <c r="A57" s="4">
         <v>44422</v>
       </c>
@@ -4695,7 +4647,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="58" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="58" spans="1:8" ht="12.75" x14ac:dyDescent="0.35">
       <c r="A58" s="4">
         <v>44423</v>
       </c>
@@ -4719,7 +4671,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="59" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="59" spans="1:8" ht="12.75" x14ac:dyDescent="0.35">
       <c r="A59" s="4">
         <v>44424</v>
       </c>
@@ -4743,7 +4695,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="60" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="60" spans="1:8" ht="12.75" x14ac:dyDescent="0.35">
       <c r="A60" s="4">
         <v>44425</v>
       </c>
@@ -4767,7 +4719,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="61" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="61" spans="1:8" ht="12.75" x14ac:dyDescent="0.35">
       <c r="A61" s="4">
         <v>44426</v>
       </c>
@@ -4791,7 +4743,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="62" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="62" spans="1:8" ht="12.75" x14ac:dyDescent="0.35">
       <c r="A62" s="4">
         <v>44427</v>
       </c>
@@ -4815,7 +4767,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="63" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="63" spans="1:8" ht="12.75" x14ac:dyDescent="0.35">
       <c r="A63" s="4">
         <v>44428</v>
       </c>
@@ -4839,7 +4791,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="64" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="64" spans="1:8" ht="12.75" x14ac:dyDescent="0.35">
       <c r="A64" s="4">
         <v>44429</v>
       </c>
@@ -4863,7 +4815,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="65" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="65" spans="1:8" ht="12.75" x14ac:dyDescent="0.35">
       <c r="A65" s="4">
         <v>44430</v>
       </c>
@@ -4887,7 +4839,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="66" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="66" spans="1:8" ht="12.75" x14ac:dyDescent="0.35">
       <c r="A66" s="4">
         <v>44431</v>
       </c>
@@ -4911,7 +4863,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="67" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="67" spans="1:8" ht="12.75" x14ac:dyDescent="0.35">
       <c r="A67" s="4">
         <v>44432</v>
       </c>
@@ -4935,7 +4887,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="68" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="68" spans="1:8" ht="12.75" x14ac:dyDescent="0.35">
       <c r="A68" s="4">
         <v>44433</v>
       </c>
@@ -4959,7 +4911,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="69" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="69" spans="1:8" ht="12.75" x14ac:dyDescent="0.35">
       <c r="A69" s="4">
         <v>44434</v>
       </c>
@@ -4983,7 +4935,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="70" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="70" spans="1:8" ht="12.75" x14ac:dyDescent="0.35">
       <c r="A70" s="4">
         <v>44435</v>
       </c>
@@ -5007,7 +4959,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="71" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="71" spans="1:8" ht="12.75" x14ac:dyDescent="0.35">
       <c r="A71" s="4">
         <v>44436</v>
       </c>
@@ -5031,7 +4983,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="72" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="72" spans="1:8" ht="12.75" x14ac:dyDescent="0.35">
       <c r="A72" s="4">
         <v>44437</v>
       </c>
@@ -5056,7 +5008,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="73" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="73" spans="1:8" ht="12.75" x14ac:dyDescent="0.35">
       <c r="A73" s="4">
         <v>44438</v>
       </c>
@@ -5081,7 +5033,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="74" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="74" spans="1:8" ht="12.75" x14ac:dyDescent="0.35">
       <c r="A74" s="4">
         <v>44439</v>
       </c>
@@ -5105,7 +5057,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="75" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="75" spans="1:8" ht="12.75" x14ac:dyDescent="0.35">
       <c r="A75" s="4">
         <v>44440</v>
       </c>
@@ -5129,7 +5081,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="76" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="76" spans="1:8" ht="12.75" x14ac:dyDescent="0.35">
       <c r="A76" s="4">
         <v>44441</v>
       </c>
@@ -5153,7 +5105,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="77" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="77" spans="1:8" ht="12.75" x14ac:dyDescent="0.35">
       <c r="A77" s="4">
         <v>44442</v>
       </c>
@@ -5177,7 +5129,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="78" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="78" spans="1:8" ht="12.75" x14ac:dyDescent="0.35">
       <c r="A78" s="4">
         <v>44443</v>
       </c>
@@ -5201,7 +5153,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="79" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="79" spans="1:8" ht="12.75" x14ac:dyDescent="0.35">
       <c r="A79" s="4">
         <v>44444</v>
       </c>
@@ -5225,7 +5177,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="80" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="80" spans="1:8" ht="12.75" x14ac:dyDescent="0.35">
       <c r="A80" s="4">
         <v>44445</v>
       </c>
@@ -5249,7 +5201,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="81" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="81" spans="1:8" ht="12.75" x14ac:dyDescent="0.35">
       <c r="A81" s="4">
         <v>44446</v>
       </c>
@@ -5273,7 +5225,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="82" spans="1:8" s="10" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="82" spans="1:8" s="10" customFormat="1" x14ac:dyDescent="0.4">
       <c r="A82" s="8" t="s">
         <v>5</v>
       </c>
@@ -5339,532 +5291,532 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <dimension ref="A1:H64"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <pane ySplit="1" topLeftCell="A62" activePane="bottomLeft" state="frozen"/>
       <selection activeCell="A2" sqref="A2"/>
-      <selection pane="bottomLeft" activeCell="A66" sqref="A66:XFD86"/>
+      <selection pane="bottomLeft" activeCell="A64" sqref="A64"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="13.2" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="13.15" x14ac:dyDescent="0.4"/>
   <cols>
-    <col min="1" max="1" width="11.3984375" style="14" customWidth="1"/>
-    <col min="2" max="2" width="9.59765625" style="12" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="11.375" style="14" customWidth="1"/>
+    <col min="2" max="2" width="9.625" style="12" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="9" style="12" bestFit="1" customWidth="1"/>
-    <col min="4" max="5" width="8.59765625" style="12" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="9.59765625" style="10" customWidth="1"/>
-    <col min="7" max="7" width="3.59765625" style="7" customWidth="1"/>
+    <col min="4" max="5" width="8.625" style="12" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="9.625" style="10" customWidth="1"/>
+    <col min="7" max="7" width="3.625" style="7" customWidth="1"/>
     <col min="8" max="8" width="9" style="12" bestFit="1" customWidth="1"/>
     <col min="9" max="256" width="9" style="7"/>
-    <col min="257" max="257" width="11.3984375" style="7" customWidth="1"/>
-    <col min="258" max="258" width="9.59765625" style="7" bestFit="1" customWidth="1"/>
+    <col min="257" max="257" width="11.375" style="7" customWidth="1"/>
+    <col min="258" max="258" width="9.625" style="7" bestFit="1" customWidth="1"/>
     <col min="259" max="259" width="9" style="7" bestFit="1" customWidth="1"/>
-    <col min="260" max="261" width="8.59765625" style="7" bestFit="1" customWidth="1"/>
-    <col min="262" max="262" width="9.59765625" style="7" customWidth="1"/>
+    <col min="260" max="261" width="8.625" style="7" bestFit="1" customWidth="1"/>
+    <col min="262" max="262" width="9.625" style="7" customWidth="1"/>
     <col min="263" max="263" width="9" style="7"/>
     <col min="264" max="264" width="9" style="7" bestFit="1" customWidth="1"/>
     <col min="265" max="512" width="9" style="7"/>
-    <col min="513" max="513" width="11.3984375" style="7" customWidth="1"/>
-    <col min="514" max="514" width="9.59765625" style="7" bestFit="1" customWidth="1"/>
+    <col min="513" max="513" width="11.375" style="7" customWidth="1"/>
+    <col min="514" max="514" width="9.625" style="7" bestFit="1" customWidth="1"/>
     <col min="515" max="515" width="9" style="7" bestFit="1" customWidth="1"/>
-    <col min="516" max="517" width="8.59765625" style="7" bestFit="1" customWidth="1"/>
-    <col min="518" max="518" width="9.59765625" style="7" customWidth="1"/>
+    <col min="516" max="517" width="8.625" style="7" bestFit="1" customWidth="1"/>
+    <col min="518" max="518" width="9.625" style="7" customWidth="1"/>
     <col min="519" max="519" width="9" style="7"/>
     <col min="520" max="520" width="9" style="7" bestFit="1" customWidth="1"/>
     <col min="521" max="768" width="9" style="7"/>
-    <col min="769" max="769" width="11.3984375" style="7" customWidth="1"/>
-    <col min="770" max="770" width="9.59765625" style="7" bestFit="1" customWidth="1"/>
+    <col min="769" max="769" width="11.375" style="7" customWidth="1"/>
+    <col min="770" max="770" width="9.625" style="7" bestFit="1" customWidth="1"/>
     <col min="771" max="771" width="9" style="7" bestFit="1" customWidth="1"/>
-    <col min="772" max="773" width="8.59765625" style="7" bestFit="1" customWidth="1"/>
-    <col min="774" max="774" width="9.59765625" style="7" customWidth="1"/>
+    <col min="772" max="773" width="8.625" style="7" bestFit="1" customWidth="1"/>
+    <col min="774" max="774" width="9.625" style="7" customWidth="1"/>
     <col min="775" max="775" width="9" style="7"/>
     <col min="776" max="776" width="9" style="7" bestFit="1" customWidth="1"/>
     <col min="777" max="1024" width="9" style="7"/>
-    <col min="1025" max="1025" width="11.3984375" style="7" customWidth="1"/>
-    <col min="1026" max="1026" width="9.59765625" style="7" bestFit="1" customWidth="1"/>
+    <col min="1025" max="1025" width="11.375" style="7" customWidth="1"/>
+    <col min="1026" max="1026" width="9.625" style="7" bestFit="1" customWidth="1"/>
     <col min="1027" max="1027" width="9" style="7" bestFit="1" customWidth="1"/>
-    <col min="1028" max="1029" width="8.59765625" style="7" bestFit="1" customWidth="1"/>
-    <col min="1030" max="1030" width="9.59765625" style="7" customWidth="1"/>
+    <col min="1028" max="1029" width="8.625" style="7" bestFit="1" customWidth="1"/>
+    <col min="1030" max="1030" width="9.625" style="7" customWidth="1"/>
     <col min="1031" max="1031" width="9" style="7"/>
     <col min="1032" max="1032" width="9" style="7" bestFit="1" customWidth="1"/>
     <col min="1033" max="1280" width="9" style="7"/>
-    <col min="1281" max="1281" width="11.3984375" style="7" customWidth="1"/>
-    <col min="1282" max="1282" width="9.59765625" style="7" bestFit="1" customWidth="1"/>
+    <col min="1281" max="1281" width="11.375" style="7" customWidth="1"/>
+    <col min="1282" max="1282" width="9.625" style="7" bestFit="1" customWidth="1"/>
     <col min="1283" max="1283" width="9" style="7" bestFit="1" customWidth="1"/>
-    <col min="1284" max="1285" width="8.59765625" style="7" bestFit="1" customWidth="1"/>
-    <col min="1286" max="1286" width="9.59765625" style="7" customWidth="1"/>
+    <col min="1284" max="1285" width="8.625" style="7" bestFit="1" customWidth="1"/>
+    <col min="1286" max="1286" width="9.625" style="7" customWidth="1"/>
     <col min="1287" max="1287" width="9" style="7"/>
     <col min="1288" max="1288" width="9" style="7" bestFit="1" customWidth="1"/>
     <col min="1289" max="1536" width="9" style="7"/>
-    <col min="1537" max="1537" width="11.3984375" style="7" customWidth="1"/>
-    <col min="1538" max="1538" width="9.59765625" style="7" bestFit="1" customWidth="1"/>
+    <col min="1537" max="1537" width="11.375" style="7" customWidth="1"/>
+    <col min="1538" max="1538" width="9.625" style="7" bestFit="1" customWidth="1"/>
     <col min="1539" max="1539" width="9" style="7" bestFit="1" customWidth="1"/>
-    <col min="1540" max="1541" width="8.59765625" style="7" bestFit="1" customWidth="1"/>
-    <col min="1542" max="1542" width="9.59765625" style="7" customWidth="1"/>
+    <col min="1540" max="1541" width="8.625" style="7" bestFit="1" customWidth="1"/>
+    <col min="1542" max="1542" width="9.625" style="7" customWidth="1"/>
     <col min="1543" max="1543" width="9" style="7"/>
     <col min="1544" max="1544" width="9" style="7" bestFit="1" customWidth="1"/>
     <col min="1545" max="1792" width="9" style="7"/>
-    <col min="1793" max="1793" width="11.3984375" style="7" customWidth="1"/>
-    <col min="1794" max="1794" width="9.59765625" style="7" bestFit="1" customWidth="1"/>
+    <col min="1793" max="1793" width="11.375" style="7" customWidth="1"/>
+    <col min="1794" max="1794" width="9.625" style="7" bestFit="1" customWidth="1"/>
     <col min="1795" max="1795" width="9" style="7" bestFit="1" customWidth="1"/>
-    <col min="1796" max="1797" width="8.59765625" style="7" bestFit="1" customWidth="1"/>
-    <col min="1798" max="1798" width="9.59765625" style="7" customWidth="1"/>
+    <col min="1796" max="1797" width="8.625" style="7" bestFit="1" customWidth="1"/>
+    <col min="1798" max="1798" width="9.625" style="7" customWidth="1"/>
     <col min="1799" max="1799" width="9" style="7"/>
     <col min="1800" max="1800" width="9" style="7" bestFit="1" customWidth="1"/>
     <col min="1801" max="2048" width="9" style="7"/>
-    <col min="2049" max="2049" width="11.3984375" style="7" customWidth="1"/>
-    <col min="2050" max="2050" width="9.59765625" style="7" bestFit="1" customWidth="1"/>
+    <col min="2049" max="2049" width="11.375" style="7" customWidth="1"/>
+    <col min="2050" max="2050" width="9.625" style="7" bestFit="1" customWidth="1"/>
     <col min="2051" max="2051" width="9" style="7" bestFit="1" customWidth="1"/>
-    <col min="2052" max="2053" width="8.59765625" style="7" bestFit="1" customWidth="1"/>
-    <col min="2054" max="2054" width="9.59765625" style="7" customWidth="1"/>
+    <col min="2052" max="2053" width="8.625" style="7" bestFit="1" customWidth="1"/>
+    <col min="2054" max="2054" width="9.625" style="7" customWidth="1"/>
     <col min="2055" max="2055" width="9" style="7"/>
     <col min="2056" max="2056" width="9" style="7" bestFit="1" customWidth="1"/>
     <col min="2057" max="2304" width="9" style="7"/>
-    <col min="2305" max="2305" width="11.3984375" style="7" customWidth="1"/>
-    <col min="2306" max="2306" width="9.59765625" style="7" bestFit="1" customWidth="1"/>
+    <col min="2305" max="2305" width="11.375" style="7" customWidth="1"/>
+    <col min="2306" max="2306" width="9.625" style="7" bestFit="1" customWidth="1"/>
     <col min="2307" max="2307" width="9" style="7" bestFit="1" customWidth="1"/>
-    <col min="2308" max="2309" width="8.59765625" style="7" bestFit="1" customWidth="1"/>
-    <col min="2310" max="2310" width="9.59765625" style="7" customWidth="1"/>
+    <col min="2308" max="2309" width="8.625" style="7" bestFit="1" customWidth="1"/>
+    <col min="2310" max="2310" width="9.625" style="7" customWidth="1"/>
     <col min="2311" max="2311" width="9" style="7"/>
     <col min="2312" max="2312" width="9" style="7" bestFit="1" customWidth="1"/>
     <col min="2313" max="2560" width="9" style="7"/>
-    <col min="2561" max="2561" width="11.3984375" style="7" customWidth="1"/>
-    <col min="2562" max="2562" width="9.59765625" style="7" bestFit="1" customWidth="1"/>
+    <col min="2561" max="2561" width="11.375" style="7" customWidth="1"/>
+    <col min="2562" max="2562" width="9.625" style="7" bestFit="1" customWidth="1"/>
     <col min="2563" max="2563" width="9" style="7" bestFit="1" customWidth="1"/>
-    <col min="2564" max="2565" width="8.59765625" style="7" bestFit="1" customWidth="1"/>
-    <col min="2566" max="2566" width="9.59765625" style="7" customWidth="1"/>
+    <col min="2564" max="2565" width="8.625" style="7" bestFit="1" customWidth="1"/>
+    <col min="2566" max="2566" width="9.625" style="7" customWidth="1"/>
     <col min="2567" max="2567" width="9" style="7"/>
     <col min="2568" max="2568" width="9" style="7" bestFit="1" customWidth="1"/>
     <col min="2569" max="2816" width="9" style="7"/>
-    <col min="2817" max="2817" width="11.3984375" style="7" customWidth="1"/>
-    <col min="2818" max="2818" width="9.59765625" style="7" bestFit="1" customWidth="1"/>
+    <col min="2817" max="2817" width="11.375" style="7" customWidth="1"/>
+    <col min="2818" max="2818" width="9.625" style="7" bestFit="1" customWidth="1"/>
     <col min="2819" max="2819" width="9" style="7" bestFit="1" customWidth="1"/>
-    <col min="2820" max="2821" width="8.59765625" style="7" bestFit="1" customWidth="1"/>
-    <col min="2822" max="2822" width="9.59765625" style="7" customWidth="1"/>
+    <col min="2820" max="2821" width="8.625" style="7" bestFit="1" customWidth="1"/>
+    <col min="2822" max="2822" width="9.625" style="7" customWidth="1"/>
     <col min="2823" max="2823" width="9" style="7"/>
     <col min="2824" max="2824" width="9" style="7" bestFit="1" customWidth="1"/>
     <col min="2825" max="3072" width="9" style="7"/>
-    <col min="3073" max="3073" width="11.3984375" style="7" customWidth="1"/>
-    <col min="3074" max="3074" width="9.59765625" style="7" bestFit="1" customWidth="1"/>
+    <col min="3073" max="3073" width="11.375" style="7" customWidth="1"/>
+    <col min="3074" max="3074" width="9.625" style="7" bestFit="1" customWidth="1"/>
     <col min="3075" max="3075" width="9" style="7" bestFit="1" customWidth="1"/>
-    <col min="3076" max="3077" width="8.59765625" style="7" bestFit="1" customWidth="1"/>
-    <col min="3078" max="3078" width="9.59765625" style="7" customWidth="1"/>
+    <col min="3076" max="3077" width="8.625" style="7" bestFit="1" customWidth="1"/>
+    <col min="3078" max="3078" width="9.625" style="7" customWidth="1"/>
     <col min="3079" max="3079" width="9" style="7"/>
     <col min="3080" max="3080" width="9" style="7" bestFit="1" customWidth="1"/>
     <col min="3081" max="3328" width="9" style="7"/>
-    <col min="3329" max="3329" width="11.3984375" style="7" customWidth="1"/>
-    <col min="3330" max="3330" width="9.59765625" style="7" bestFit="1" customWidth="1"/>
+    <col min="3329" max="3329" width="11.375" style="7" customWidth="1"/>
+    <col min="3330" max="3330" width="9.625" style="7" bestFit="1" customWidth="1"/>
     <col min="3331" max="3331" width="9" style="7" bestFit="1" customWidth="1"/>
-    <col min="3332" max="3333" width="8.59765625" style="7" bestFit="1" customWidth="1"/>
-    <col min="3334" max="3334" width="9.59765625" style="7" customWidth="1"/>
+    <col min="3332" max="3333" width="8.625" style="7" bestFit="1" customWidth="1"/>
+    <col min="3334" max="3334" width="9.625" style="7" customWidth="1"/>
     <col min="3335" max="3335" width="9" style="7"/>
     <col min="3336" max="3336" width="9" style="7" bestFit="1" customWidth="1"/>
     <col min="3337" max="3584" width="9" style="7"/>
-    <col min="3585" max="3585" width="11.3984375" style="7" customWidth="1"/>
-    <col min="3586" max="3586" width="9.59765625" style="7" bestFit="1" customWidth="1"/>
+    <col min="3585" max="3585" width="11.375" style="7" customWidth="1"/>
+    <col min="3586" max="3586" width="9.625" style="7" bestFit="1" customWidth="1"/>
     <col min="3587" max="3587" width="9" style="7" bestFit="1" customWidth="1"/>
-    <col min="3588" max="3589" width="8.59765625" style="7" bestFit="1" customWidth="1"/>
-    <col min="3590" max="3590" width="9.59765625" style="7" customWidth="1"/>
+    <col min="3588" max="3589" width="8.625" style="7" bestFit="1" customWidth="1"/>
+    <col min="3590" max="3590" width="9.625" style="7" customWidth="1"/>
     <col min="3591" max="3591" width="9" style="7"/>
     <col min="3592" max="3592" width="9" style="7" bestFit="1" customWidth="1"/>
     <col min="3593" max="3840" width="9" style="7"/>
-    <col min="3841" max="3841" width="11.3984375" style="7" customWidth="1"/>
-    <col min="3842" max="3842" width="9.59765625" style="7" bestFit="1" customWidth="1"/>
+    <col min="3841" max="3841" width="11.375" style="7" customWidth="1"/>
+    <col min="3842" max="3842" width="9.625" style="7" bestFit="1" customWidth="1"/>
     <col min="3843" max="3843" width="9" style="7" bestFit="1" customWidth="1"/>
-    <col min="3844" max="3845" width="8.59765625" style="7" bestFit="1" customWidth="1"/>
-    <col min="3846" max="3846" width="9.59765625" style="7" customWidth="1"/>
+    <col min="3844" max="3845" width="8.625" style="7" bestFit="1" customWidth="1"/>
+    <col min="3846" max="3846" width="9.625" style="7" customWidth="1"/>
     <col min="3847" max="3847" width="9" style="7"/>
     <col min="3848" max="3848" width="9" style="7" bestFit="1" customWidth="1"/>
     <col min="3849" max="4096" width="9" style="7"/>
-    <col min="4097" max="4097" width="11.3984375" style="7" customWidth="1"/>
-    <col min="4098" max="4098" width="9.59765625" style="7" bestFit="1" customWidth="1"/>
+    <col min="4097" max="4097" width="11.375" style="7" customWidth="1"/>
+    <col min="4098" max="4098" width="9.625" style="7" bestFit="1" customWidth="1"/>
     <col min="4099" max="4099" width="9" style="7" bestFit="1" customWidth="1"/>
-    <col min="4100" max="4101" width="8.59765625" style="7" bestFit="1" customWidth="1"/>
-    <col min="4102" max="4102" width="9.59765625" style="7" customWidth="1"/>
+    <col min="4100" max="4101" width="8.625" style="7" bestFit="1" customWidth="1"/>
+    <col min="4102" max="4102" width="9.625" style="7" customWidth="1"/>
     <col min="4103" max="4103" width="9" style="7"/>
     <col min="4104" max="4104" width="9" style="7" bestFit="1" customWidth="1"/>
     <col min="4105" max="4352" width="9" style="7"/>
-    <col min="4353" max="4353" width="11.3984375" style="7" customWidth="1"/>
-    <col min="4354" max="4354" width="9.59765625" style="7" bestFit="1" customWidth="1"/>
+    <col min="4353" max="4353" width="11.375" style="7" customWidth="1"/>
+    <col min="4354" max="4354" width="9.625" style="7" bestFit="1" customWidth="1"/>
     <col min="4355" max="4355" width="9" style="7" bestFit="1" customWidth="1"/>
-    <col min="4356" max="4357" width="8.59765625" style="7" bestFit="1" customWidth="1"/>
-    <col min="4358" max="4358" width="9.59765625" style="7" customWidth="1"/>
+    <col min="4356" max="4357" width="8.625" style="7" bestFit="1" customWidth="1"/>
+    <col min="4358" max="4358" width="9.625" style="7" customWidth="1"/>
     <col min="4359" max="4359" width="9" style="7"/>
     <col min="4360" max="4360" width="9" style="7" bestFit="1" customWidth="1"/>
     <col min="4361" max="4608" width="9" style="7"/>
-    <col min="4609" max="4609" width="11.3984375" style="7" customWidth="1"/>
-    <col min="4610" max="4610" width="9.59765625" style="7" bestFit="1" customWidth="1"/>
+    <col min="4609" max="4609" width="11.375" style="7" customWidth="1"/>
+    <col min="4610" max="4610" width="9.625" style="7" bestFit="1" customWidth="1"/>
     <col min="4611" max="4611" width="9" style="7" bestFit="1" customWidth="1"/>
-    <col min="4612" max="4613" width="8.59765625" style="7" bestFit="1" customWidth="1"/>
-    <col min="4614" max="4614" width="9.59765625" style="7" customWidth="1"/>
+    <col min="4612" max="4613" width="8.625" style="7" bestFit="1" customWidth="1"/>
+    <col min="4614" max="4614" width="9.625" style="7" customWidth="1"/>
     <col min="4615" max="4615" width="9" style="7"/>
     <col min="4616" max="4616" width="9" style="7" bestFit="1" customWidth="1"/>
     <col min="4617" max="4864" width="9" style="7"/>
-    <col min="4865" max="4865" width="11.3984375" style="7" customWidth="1"/>
-    <col min="4866" max="4866" width="9.59765625" style="7" bestFit="1" customWidth="1"/>
+    <col min="4865" max="4865" width="11.375" style="7" customWidth="1"/>
+    <col min="4866" max="4866" width="9.625" style="7" bestFit="1" customWidth="1"/>
     <col min="4867" max="4867" width="9" style="7" bestFit="1" customWidth="1"/>
-    <col min="4868" max="4869" width="8.59765625" style="7" bestFit="1" customWidth="1"/>
-    <col min="4870" max="4870" width="9.59765625" style="7" customWidth="1"/>
+    <col min="4868" max="4869" width="8.625" style="7" bestFit="1" customWidth="1"/>
+    <col min="4870" max="4870" width="9.625" style="7" customWidth="1"/>
     <col min="4871" max="4871" width="9" style="7"/>
     <col min="4872" max="4872" width="9" style="7" bestFit="1" customWidth="1"/>
     <col min="4873" max="5120" width="9" style="7"/>
-    <col min="5121" max="5121" width="11.3984375" style="7" customWidth="1"/>
-    <col min="5122" max="5122" width="9.59765625" style="7" bestFit="1" customWidth="1"/>
+    <col min="5121" max="5121" width="11.375" style="7" customWidth="1"/>
+    <col min="5122" max="5122" width="9.625" style="7" bestFit="1" customWidth="1"/>
     <col min="5123" max="5123" width="9" style="7" bestFit="1" customWidth="1"/>
-    <col min="5124" max="5125" width="8.59765625" style="7" bestFit="1" customWidth="1"/>
-    <col min="5126" max="5126" width="9.59765625" style="7" customWidth="1"/>
+    <col min="5124" max="5125" width="8.625" style="7" bestFit="1" customWidth="1"/>
+    <col min="5126" max="5126" width="9.625" style="7" customWidth="1"/>
     <col min="5127" max="5127" width="9" style="7"/>
     <col min="5128" max="5128" width="9" style="7" bestFit="1" customWidth="1"/>
     <col min="5129" max="5376" width="9" style="7"/>
-    <col min="5377" max="5377" width="11.3984375" style="7" customWidth="1"/>
-    <col min="5378" max="5378" width="9.59765625" style="7" bestFit="1" customWidth="1"/>
+    <col min="5377" max="5377" width="11.375" style="7" customWidth="1"/>
+    <col min="5378" max="5378" width="9.625" style="7" bestFit="1" customWidth="1"/>
     <col min="5379" max="5379" width="9" style="7" bestFit="1" customWidth="1"/>
-    <col min="5380" max="5381" width="8.59765625" style="7" bestFit="1" customWidth="1"/>
-    <col min="5382" max="5382" width="9.59765625" style="7" customWidth="1"/>
+    <col min="5380" max="5381" width="8.625" style="7" bestFit="1" customWidth="1"/>
+    <col min="5382" max="5382" width="9.625" style="7" customWidth="1"/>
     <col min="5383" max="5383" width="9" style="7"/>
     <col min="5384" max="5384" width="9" style="7" bestFit="1" customWidth="1"/>
     <col min="5385" max="5632" width="9" style="7"/>
-    <col min="5633" max="5633" width="11.3984375" style="7" customWidth="1"/>
-    <col min="5634" max="5634" width="9.59765625" style="7" bestFit="1" customWidth="1"/>
+    <col min="5633" max="5633" width="11.375" style="7" customWidth="1"/>
+    <col min="5634" max="5634" width="9.625" style="7" bestFit="1" customWidth="1"/>
     <col min="5635" max="5635" width="9" style="7" bestFit="1" customWidth="1"/>
-    <col min="5636" max="5637" width="8.59765625" style="7" bestFit="1" customWidth="1"/>
-    <col min="5638" max="5638" width="9.59765625" style="7" customWidth="1"/>
+    <col min="5636" max="5637" width="8.625" style="7" bestFit="1" customWidth="1"/>
+    <col min="5638" max="5638" width="9.625" style="7" customWidth="1"/>
     <col min="5639" max="5639" width="9" style="7"/>
     <col min="5640" max="5640" width="9" style="7" bestFit="1" customWidth="1"/>
     <col min="5641" max="5888" width="9" style="7"/>
-    <col min="5889" max="5889" width="11.3984375" style="7" customWidth="1"/>
-    <col min="5890" max="5890" width="9.59765625" style="7" bestFit="1" customWidth="1"/>
+    <col min="5889" max="5889" width="11.375" style="7" customWidth="1"/>
+    <col min="5890" max="5890" width="9.625" style="7" bestFit="1" customWidth="1"/>
     <col min="5891" max="5891" width="9" style="7" bestFit="1" customWidth="1"/>
-    <col min="5892" max="5893" width="8.59765625" style="7" bestFit="1" customWidth="1"/>
-    <col min="5894" max="5894" width="9.59765625" style="7" customWidth="1"/>
+    <col min="5892" max="5893" width="8.625" style="7" bestFit="1" customWidth="1"/>
+    <col min="5894" max="5894" width="9.625" style="7" customWidth="1"/>
     <col min="5895" max="5895" width="9" style="7"/>
     <col min="5896" max="5896" width="9" style="7" bestFit="1" customWidth="1"/>
     <col min="5897" max="6144" width="9" style="7"/>
-    <col min="6145" max="6145" width="11.3984375" style="7" customWidth="1"/>
-    <col min="6146" max="6146" width="9.59765625" style="7" bestFit="1" customWidth="1"/>
+    <col min="6145" max="6145" width="11.375" style="7" customWidth="1"/>
+    <col min="6146" max="6146" width="9.625" style="7" bestFit="1" customWidth="1"/>
     <col min="6147" max="6147" width="9" style="7" bestFit="1" customWidth="1"/>
-    <col min="6148" max="6149" width="8.59765625" style="7" bestFit="1" customWidth="1"/>
-    <col min="6150" max="6150" width="9.59765625" style="7" customWidth="1"/>
+    <col min="6148" max="6149" width="8.625" style="7" bestFit="1" customWidth="1"/>
+    <col min="6150" max="6150" width="9.625" style="7" customWidth="1"/>
     <col min="6151" max="6151" width="9" style="7"/>
     <col min="6152" max="6152" width="9" style="7" bestFit="1" customWidth="1"/>
     <col min="6153" max="6400" width="9" style="7"/>
-    <col min="6401" max="6401" width="11.3984375" style="7" customWidth="1"/>
-    <col min="6402" max="6402" width="9.59765625" style="7" bestFit="1" customWidth="1"/>
+    <col min="6401" max="6401" width="11.375" style="7" customWidth="1"/>
+    <col min="6402" max="6402" width="9.625" style="7" bestFit="1" customWidth="1"/>
     <col min="6403" max="6403" width="9" style="7" bestFit="1" customWidth="1"/>
-    <col min="6404" max="6405" width="8.59765625" style="7" bestFit="1" customWidth="1"/>
-    <col min="6406" max="6406" width="9.59765625" style="7" customWidth="1"/>
+    <col min="6404" max="6405" width="8.625" style="7" bestFit="1" customWidth="1"/>
+    <col min="6406" max="6406" width="9.625" style="7" customWidth="1"/>
     <col min="6407" max="6407" width="9" style="7"/>
     <col min="6408" max="6408" width="9" style="7" bestFit="1" customWidth="1"/>
     <col min="6409" max="6656" width="9" style="7"/>
-    <col min="6657" max="6657" width="11.3984375" style="7" customWidth="1"/>
-    <col min="6658" max="6658" width="9.59765625" style="7" bestFit="1" customWidth="1"/>
+    <col min="6657" max="6657" width="11.375" style="7" customWidth="1"/>
+    <col min="6658" max="6658" width="9.625" style="7" bestFit="1" customWidth="1"/>
     <col min="6659" max="6659" width="9" style="7" bestFit="1" customWidth="1"/>
-    <col min="6660" max="6661" width="8.59765625" style="7" bestFit="1" customWidth="1"/>
-    <col min="6662" max="6662" width="9.59765625" style="7" customWidth="1"/>
+    <col min="6660" max="6661" width="8.625" style="7" bestFit="1" customWidth="1"/>
+    <col min="6662" max="6662" width="9.625" style="7" customWidth="1"/>
     <col min="6663" max="6663" width="9" style="7"/>
     <col min="6664" max="6664" width="9" style="7" bestFit="1" customWidth="1"/>
     <col min="6665" max="6912" width="9" style="7"/>
-    <col min="6913" max="6913" width="11.3984375" style="7" customWidth="1"/>
-    <col min="6914" max="6914" width="9.59765625" style="7" bestFit="1" customWidth="1"/>
+    <col min="6913" max="6913" width="11.375" style="7" customWidth="1"/>
+    <col min="6914" max="6914" width="9.625" style="7" bestFit="1" customWidth="1"/>
     <col min="6915" max="6915" width="9" style="7" bestFit="1" customWidth="1"/>
-    <col min="6916" max="6917" width="8.59765625" style="7" bestFit="1" customWidth="1"/>
-    <col min="6918" max="6918" width="9.59765625" style="7" customWidth="1"/>
+    <col min="6916" max="6917" width="8.625" style="7" bestFit="1" customWidth="1"/>
+    <col min="6918" max="6918" width="9.625" style="7" customWidth="1"/>
     <col min="6919" max="6919" width="9" style="7"/>
     <col min="6920" max="6920" width="9" style="7" bestFit="1" customWidth="1"/>
     <col min="6921" max="7168" width="9" style="7"/>
-    <col min="7169" max="7169" width="11.3984375" style="7" customWidth="1"/>
-    <col min="7170" max="7170" width="9.59765625" style="7" bestFit="1" customWidth="1"/>
+    <col min="7169" max="7169" width="11.375" style="7" customWidth="1"/>
+    <col min="7170" max="7170" width="9.625" style="7" bestFit="1" customWidth="1"/>
     <col min="7171" max="7171" width="9" style="7" bestFit="1" customWidth="1"/>
-    <col min="7172" max="7173" width="8.59765625" style="7" bestFit="1" customWidth="1"/>
-    <col min="7174" max="7174" width="9.59765625" style="7" customWidth="1"/>
+    <col min="7172" max="7173" width="8.625" style="7" bestFit="1" customWidth="1"/>
+    <col min="7174" max="7174" width="9.625" style="7" customWidth="1"/>
     <col min="7175" max="7175" width="9" style="7"/>
     <col min="7176" max="7176" width="9" style="7" bestFit="1" customWidth="1"/>
     <col min="7177" max="7424" width="9" style="7"/>
-    <col min="7425" max="7425" width="11.3984375" style="7" customWidth="1"/>
-    <col min="7426" max="7426" width="9.59765625" style="7" bestFit="1" customWidth="1"/>
+    <col min="7425" max="7425" width="11.375" style="7" customWidth="1"/>
+    <col min="7426" max="7426" width="9.625" style="7" bestFit="1" customWidth="1"/>
     <col min="7427" max="7427" width="9" style="7" bestFit="1" customWidth="1"/>
-    <col min="7428" max="7429" width="8.59765625" style="7" bestFit="1" customWidth="1"/>
-    <col min="7430" max="7430" width="9.59765625" style="7" customWidth="1"/>
+    <col min="7428" max="7429" width="8.625" style="7" bestFit="1" customWidth="1"/>
+    <col min="7430" max="7430" width="9.625" style="7" customWidth="1"/>
     <col min="7431" max="7431" width="9" style="7"/>
     <col min="7432" max="7432" width="9" style="7" bestFit="1" customWidth="1"/>
     <col min="7433" max="7680" width="9" style="7"/>
-    <col min="7681" max="7681" width="11.3984375" style="7" customWidth="1"/>
-    <col min="7682" max="7682" width="9.59765625" style="7" bestFit="1" customWidth="1"/>
+    <col min="7681" max="7681" width="11.375" style="7" customWidth="1"/>
+    <col min="7682" max="7682" width="9.625" style="7" bestFit="1" customWidth="1"/>
     <col min="7683" max="7683" width="9" style="7" bestFit="1" customWidth="1"/>
-    <col min="7684" max="7685" width="8.59765625" style="7" bestFit="1" customWidth="1"/>
-    <col min="7686" max="7686" width="9.59765625" style="7" customWidth="1"/>
+    <col min="7684" max="7685" width="8.625" style="7" bestFit="1" customWidth="1"/>
+    <col min="7686" max="7686" width="9.625" style="7" customWidth="1"/>
     <col min="7687" max="7687" width="9" style="7"/>
     <col min="7688" max="7688" width="9" style="7" bestFit="1" customWidth="1"/>
     <col min="7689" max="7936" width="9" style="7"/>
-    <col min="7937" max="7937" width="11.3984375" style="7" customWidth="1"/>
-    <col min="7938" max="7938" width="9.59765625" style="7" bestFit="1" customWidth="1"/>
+    <col min="7937" max="7937" width="11.375" style="7" customWidth="1"/>
+    <col min="7938" max="7938" width="9.625" style="7" bestFit="1" customWidth="1"/>
     <col min="7939" max="7939" width="9" style="7" bestFit="1" customWidth="1"/>
-    <col min="7940" max="7941" width="8.59765625" style="7" bestFit="1" customWidth="1"/>
-    <col min="7942" max="7942" width="9.59765625" style="7" customWidth="1"/>
+    <col min="7940" max="7941" width="8.625" style="7" bestFit="1" customWidth="1"/>
+    <col min="7942" max="7942" width="9.625" style="7" customWidth="1"/>
     <col min="7943" max="7943" width="9" style="7"/>
     <col min="7944" max="7944" width="9" style="7" bestFit="1" customWidth="1"/>
     <col min="7945" max="8192" width="9" style="7"/>
-    <col min="8193" max="8193" width="11.3984375" style="7" customWidth="1"/>
-    <col min="8194" max="8194" width="9.59765625" style="7" bestFit="1" customWidth="1"/>
+    <col min="8193" max="8193" width="11.375" style="7" customWidth="1"/>
+    <col min="8194" max="8194" width="9.625" style="7" bestFit="1" customWidth="1"/>
     <col min="8195" max="8195" width="9" style="7" bestFit="1" customWidth="1"/>
-    <col min="8196" max="8197" width="8.59765625" style="7" bestFit="1" customWidth="1"/>
-    <col min="8198" max="8198" width="9.59765625" style="7" customWidth="1"/>
+    <col min="8196" max="8197" width="8.625" style="7" bestFit="1" customWidth="1"/>
+    <col min="8198" max="8198" width="9.625" style="7" customWidth="1"/>
     <col min="8199" max="8199" width="9" style="7"/>
     <col min="8200" max="8200" width="9" style="7" bestFit="1" customWidth="1"/>
     <col min="8201" max="8448" width="9" style="7"/>
-    <col min="8449" max="8449" width="11.3984375" style="7" customWidth="1"/>
-    <col min="8450" max="8450" width="9.59765625" style="7" bestFit="1" customWidth="1"/>
+    <col min="8449" max="8449" width="11.375" style="7" customWidth="1"/>
+    <col min="8450" max="8450" width="9.625" style="7" bestFit="1" customWidth="1"/>
     <col min="8451" max="8451" width="9" style="7" bestFit="1" customWidth="1"/>
-    <col min="8452" max="8453" width="8.59765625" style="7" bestFit="1" customWidth="1"/>
-    <col min="8454" max="8454" width="9.59765625" style="7" customWidth="1"/>
+    <col min="8452" max="8453" width="8.625" style="7" bestFit="1" customWidth="1"/>
+    <col min="8454" max="8454" width="9.625" style="7" customWidth="1"/>
     <col min="8455" max="8455" width="9" style="7"/>
     <col min="8456" max="8456" width="9" style="7" bestFit="1" customWidth="1"/>
     <col min="8457" max="8704" width="9" style="7"/>
-    <col min="8705" max="8705" width="11.3984375" style="7" customWidth="1"/>
-    <col min="8706" max="8706" width="9.59765625" style="7" bestFit="1" customWidth="1"/>
+    <col min="8705" max="8705" width="11.375" style="7" customWidth="1"/>
+    <col min="8706" max="8706" width="9.625" style="7" bestFit="1" customWidth="1"/>
     <col min="8707" max="8707" width="9" style="7" bestFit="1" customWidth="1"/>
-    <col min="8708" max="8709" width="8.59765625" style="7" bestFit="1" customWidth="1"/>
-    <col min="8710" max="8710" width="9.59765625" style="7" customWidth="1"/>
+    <col min="8708" max="8709" width="8.625" style="7" bestFit="1" customWidth="1"/>
+    <col min="8710" max="8710" width="9.625" style="7" customWidth="1"/>
     <col min="8711" max="8711" width="9" style="7"/>
     <col min="8712" max="8712" width="9" style="7" bestFit="1" customWidth="1"/>
     <col min="8713" max="8960" width="9" style="7"/>
-    <col min="8961" max="8961" width="11.3984375" style="7" customWidth="1"/>
-    <col min="8962" max="8962" width="9.59765625" style="7" bestFit="1" customWidth="1"/>
+    <col min="8961" max="8961" width="11.375" style="7" customWidth="1"/>
+    <col min="8962" max="8962" width="9.625" style="7" bestFit="1" customWidth="1"/>
     <col min="8963" max="8963" width="9" style="7" bestFit="1" customWidth="1"/>
-    <col min="8964" max="8965" width="8.59765625" style="7" bestFit="1" customWidth="1"/>
-    <col min="8966" max="8966" width="9.59765625" style="7" customWidth="1"/>
+    <col min="8964" max="8965" width="8.625" style="7" bestFit="1" customWidth="1"/>
+    <col min="8966" max="8966" width="9.625" style="7" customWidth="1"/>
     <col min="8967" max="8967" width="9" style="7"/>
     <col min="8968" max="8968" width="9" style="7" bestFit="1" customWidth="1"/>
     <col min="8969" max="9216" width="9" style="7"/>
-    <col min="9217" max="9217" width="11.3984375" style="7" customWidth="1"/>
-    <col min="9218" max="9218" width="9.59765625" style="7" bestFit="1" customWidth="1"/>
+    <col min="9217" max="9217" width="11.375" style="7" customWidth="1"/>
+    <col min="9218" max="9218" width="9.625" style="7" bestFit="1" customWidth="1"/>
     <col min="9219" max="9219" width="9" style="7" bestFit="1" customWidth="1"/>
-    <col min="9220" max="9221" width="8.59765625" style="7" bestFit="1" customWidth="1"/>
-    <col min="9222" max="9222" width="9.59765625" style="7" customWidth="1"/>
+    <col min="9220" max="9221" width="8.625" style="7" bestFit="1" customWidth="1"/>
+    <col min="9222" max="9222" width="9.625" style="7" customWidth="1"/>
     <col min="9223" max="9223" width="9" style="7"/>
     <col min="9224" max="9224" width="9" style="7" bestFit="1" customWidth="1"/>
     <col min="9225" max="9472" width="9" style="7"/>
-    <col min="9473" max="9473" width="11.3984375" style="7" customWidth="1"/>
-    <col min="9474" max="9474" width="9.59765625" style="7" bestFit="1" customWidth="1"/>
+    <col min="9473" max="9473" width="11.375" style="7" customWidth="1"/>
+    <col min="9474" max="9474" width="9.625" style="7" bestFit="1" customWidth="1"/>
     <col min="9475" max="9475" width="9" style="7" bestFit="1" customWidth="1"/>
-    <col min="9476" max="9477" width="8.59765625" style="7" bestFit="1" customWidth="1"/>
-    <col min="9478" max="9478" width="9.59765625" style="7" customWidth="1"/>
+    <col min="9476" max="9477" width="8.625" style="7" bestFit="1" customWidth="1"/>
+    <col min="9478" max="9478" width="9.625" style="7" customWidth="1"/>
     <col min="9479" max="9479" width="9" style="7"/>
     <col min="9480" max="9480" width="9" style="7" bestFit="1" customWidth="1"/>
     <col min="9481" max="9728" width="9" style="7"/>
-    <col min="9729" max="9729" width="11.3984375" style="7" customWidth="1"/>
-    <col min="9730" max="9730" width="9.59765625" style="7" bestFit="1" customWidth="1"/>
+    <col min="9729" max="9729" width="11.375" style="7" customWidth="1"/>
+    <col min="9730" max="9730" width="9.625" style="7" bestFit="1" customWidth="1"/>
     <col min="9731" max="9731" width="9" style="7" bestFit="1" customWidth="1"/>
-    <col min="9732" max="9733" width="8.59765625" style="7" bestFit="1" customWidth="1"/>
-    <col min="9734" max="9734" width="9.59765625" style="7" customWidth="1"/>
+    <col min="9732" max="9733" width="8.625" style="7" bestFit="1" customWidth="1"/>
+    <col min="9734" max="9734" width="9.625" style="7" customWidth="1"/>
     <col min="9735" max="9735" width="9" style="7"/>
     <col min="9736" max="9736" width="9" style="7" bestFit="1" customWidth="1"/>
     <col min="9737" max="9984" width="9" style="7"/>
-    <col min="9985" max="9985" width="11.3984375" style="7" customWidth="1"/>
-    <col min="9986" max="9986" width="9.59765625" style="7" bestFit="1" customWidth="1"/>
+    <col min="9985" max="9985" width="11.375" style="7" customWidth="1"/>
+    <col min="9986" max="9986" width="9.625" style="7" bestFit="1" customWidth="1"/>
     <col min="9987" max="9987" width="9" style="7" bestFit="1" customWidth="1"/>
-    <col min="9988" max="9989" width="8.59765625" style="7" bestFit="1" customWidth="1"/>
-    <col min="9990" max="9990" width="9.59765625" style="7" customWidth="1"/>
+    <col min="9988" max="9989" width="8.625" style="7" bestFit="1" customWidth="1"/>
+    <col min="9990" max="9990" width="9.625" style="7" customWidth="1"/>
     <col min="9991" max="9991" width="9" style="7"/>
     <col min="9992" max="9992" width="9" style="7" bestFit="1" customWidth="1"/>
     <col min="9993" max="10240" width="9" style="7"/>
-    <col min="10241" max="10241" width="11.3984375" style="7" customWidth="1"/>
-    <col min="10242" max="10242" width="9.59765625" style="7" bestFit="1" customWidth="1"/>
+    <col min="10241" max="10241" width="11.375" style="7" customWidth="1"/>
+    <col min="10242" max="10242" width="9.625" style="7" bestFit="1" customWidth="1"/>
     <col min="10243" max="10243" width="9" style="7" bestFit="1" customWidth="1"/>
-    <col min="10244" max="10245" width="8.59765625" style="7" bestFit="1" customWidth="1"/>
-    <col min="10246" max="10246" width="9.59765625" style="7" customWidth="1"/>
+    <col min="10244" max="10245" width="8.625" style="7" bestFit="1" customWidth="1"/>
+    <col min="10246" max="10246" width="9.625" style="7" customWidth="1"/>
     <col min="10247" max="10247" width="9" style="7"/>
     <col min="10248" max="10248" width="9" style="7" bestFit="1" customWidth="1"/>
     <col min="10249" max="10496" width="9" style="7"/>
-    <col min="10497" max="10497" width="11.3984375" style="7" customWidth="1"/>
-    <col min="10498" max="10498" width="9.59765625" style="7" bestFit="1" customWidth="1"/>
+    <col min="10497" max="10497" width="11.375" style="7" customWidth="1"/>
+    <col min="10498" max="10498" width="9.625" style="7" bestFit="1" customWidth="1"/>
     <col min="10499" max="10499" width="9" style="7" bestFit="1" customWidth="1"/>
-    <col min="10500" max="10501" width="8.59765625" style="7" bestFit="1" customWidth="1"/>
-    <col min="10502" max="10502" width="9.59765625" style="7" customWidth="1"/>
+    <col min="10500" max="10501" width="8.625" style="7" bestFit="1" customWidth="1"/>
+    <col min="10502" max="10502" width="9.625" style="7" customWidth="1"/>
     <col min="10503" max="10503" width="9" style="7"/>
     <col min="10504" max="10504" width="9" style="7" bestFit="1" customWidth="1"/>
     <col min="10505" max="10752" width="9" style="7"/>
-    <col min="10753" max="10753" width="11.3984375" style="7" customWidth="1"/>
-    <col min="10754" max="10754" width="9.59765625" style="7" bestFit="1" customWidth="1"/>
+    <col min="10753" max="10753" width="11.375" style="7" customWidth="1"/>
+    <col min="10754" max="10754" width="9.625" style="7" bestFit="1" customWidth="1"/>
     <col min="10755" max="10755" width="9" style="7" bestFit="1" customWidth="1"/>
-    <col min="10756" max="10757" width="8.59765625" style="7" bestFit="1" customWidth="1"/>
-    <col min="10758" max="10758" width="9.59765625" style="7" customWidth="1"/>
+    <col min="10756" max="10757" width="8.625" style="7" bestFit="1" customWidth="1"/>
+    <col min="10758" max="10758" width="9.625" style="7" customWidth="1"/>
     <col min="10759" max="10759" width="9" style="7"/>
     <col min="10760" max="10760" width="9" style="7" bestFit="1" customWidth="1"/>
     <col min="10761" max="11008" width="9" style="7"/>
-    <col min="11009" max="11009" width="11.3984375" style="7" customWidth="1"/>
-    <col min="11010" max="11010" width="9.59765625" style="7" bestFit="1" customWidth="1"/>
+    <col min="11009" max="11009" width="11.375" style="7" customWidth="1"/>
+    <col min="11010" max="11010" width="9.625" style="7" bestFit="1" customWidth="1"/>
     <col min="11011" max="11011" width="9" style="7" bestFit="1" customWidth="1"/>
-    <col min="11012" max="11013" width="8.59765625" style="7" bestFit="1" customWidth="1"/>
-    <col min="11014" max="11014" width="9.59765625" style="7" customWidth="1"/>
+    <col min="11012" max="11013" width="8.625" style="7" bestFit="1" customWidth="1"/>
+    <col min="11014" max="11014" width="9.625" style="7" customWidth="1"/>
     <col min="11015" max="11015" width="9" style="7"/>
     <col min="11016" max="11016" width="9" style="7" bestFit="1" customWidth="1"/>
     <col min="11017" max="11264" width="9" style="7"/>
-    <col min="11265" max="11265" width="11.3984375" style="7" customWidth="1"/>
-    <col min="11266" max="11266" width="9.59765625" style="7" bestFit="1" customWidth="1"/>
+    <col min="11265" max="11265" width="11.375" style="7" customWidth="1"/>
+    <col min="11266" max="11266" width="9.625" style="7" bestFit="1" customWidth="1"/>
     <col min="11267" max="11267" width="9" style="7" bestFit="1" customWidth="1"/>
-    <col min="11268" max="11269" width="8.59765625" style="7" bestFit="1" customWidth="1"/>
-    <col min="11270" max="11270" width="9.59765625" style="7" customWidth="1"/>
+    <col min="11268" max="11269" width="8.625" style="7" bestFit="1" customWidth="1"/>
+    <col min="11270" max="11270" width="9.625" style="7" customWidth="1"/>
     <col min="11271" max="11271" width="9" style="7"/>
     <col min="11272" max="11272" width="9" style="7" bestFit="1" customWidth="1"/>
     <col min="11273" max="11520" width="9" style="7"/>
-    <col min="11521" max="11521" width="11.3984375" style="7" customWidth="1"/>
-    <col min="11522" max="11522" width="9.59765625" style="7" bestFit="1" customWidth="1"/>
+    <col min="11521" max="11521" width="11.375" style="7" customWidth="1"/>
+    <col min="11522" max="11522" width="9.625" style="7" bestFit="1" customWidth="1"/>
     <col min="11523" max="11523" width="9" style="7" bestFit="1" customWidth="1"/>
-    <col min="11524" max="11525" width="8.59765625" style="7" bestFit="1" customWidth="1"/>
-    <col min="11526" max="11526" width="9.59765625" style="7" customWidth="1"/>
+    <col min="11524" max="11525" width="8.625" style="7" bestFit="1" customWidth="1"/>
+    <col min="11526" max="11526" width="9.625" style="7" customWidth="1"/>
     <col min="11527" max="11527" width="9" style="7"/>
     <col min="11528" max="11528" width="9" style="7" bestFit="1" customWidth="1"/>
     <col min="11529" max="11776" width="9" style="7"/>
-    <col min="11777" max="11777" width="11.3984375" style="7" customWidth="1"/>
-    <col min="11778" max="11778" width="9.59765625" style="7" bestFit="1" customWidth="1"/>
+    <col min="11777" max="11777" width="11.375" style="7" customWidth="1"/>
+    <col min="11778" max="11778" width="9.625" style="7" bestFit="1" customWidth="1"/>
     <col min="11779" max="11779" width="9" style="7" bestFit="1" customWidth="1"/>
-    <col min="11780" max="11781" width="8.59765625" style="7" bestFit="1" customWidth="1"/>
-    <col min="11782" max="11782" width="9.59765625" style="7" customWidth="1"/>
+    <col min="11780" max="11781" width="8.625" style="7" bestFit="1" customWidth="1"/>
+    <col min="11782" max="11782" width="9.625" style="7" customWidth="1"/>
     <col min="11783" max="11783" width="9" style="7"/>
     <col min="11784" max="11784" width="9" style="7" bestFit="1" customWidth="1"/>
     <col min="11785" max="12032" width="9" style="7"/>
-    <col min="12033" max="12033" width="11.3984375" style="7" customWidth="1"/>
-    <col min="12034" max="12034" width="9.59765625" style="7" bestFit="1" customWidth="1"/>
+    <col min="12033" max="12033" width="11.375" style="7" customWidth="1"/>
+    <col min="12034" max="12034" width="9.625" style="7" bestFit="1" customWidth="1"/>
     <col min="12035" max="12035" width="9" style="7" bestFit="1" customWidth="1"/>
-    <col min="12036" max="12037" width="8.59765625" style="7" bestFit="1" customWidth="1"/>
-    <col min="12038" max="12038" width="9.59765625" style="7" customWidth="1"/>
+    <col min="12036" max="12037" width="8.625" style="7" bestFit="1" customWidth="1"/>
+    <col min="12038" max="12038" width="9.625" style="7" customWidth="1"/>
     <col min="12039" max="12039" width="9" style="7"/>
     <col min="12040" max="12040" width="9" style="7" bestFit="1" customWidth="1"/>
     <col min="12041" max="12288" width="9" style="7"/>
-    <col min="12289" max="12289" width="11.3984375" style="7" customWidth="1"/>
-    <col min="12290" max="12290" width="9.59765625" style="7" bestFit="1" customWidth="1"/>
+    <col min="12289" max="12289" width="11.375" style="7" customWidth="1"/>
+    <col min="12290" max="12290" width="9.625" style="7" bestFit="1" customWidth="1"/>
     <col min="12291" max="12291" width="9" style="7" bestFit="1" customWidth="1"/>
-    <col min="12292" max="12293" width="8.59765625" style="7" bestFit="1" customWidth="1"/>
-    <col min="12294" max="12294" width="9.59765625" style="7" customWidth="1"/>
+    <col min="12292" max="12293" width="8.625" style="7" bestFit="1" customWidth="1"/>
+    <col min="12294" max="12294" width="9.625" style="7" customWidth="1"/>
     <col min="12295" max="12295" width="9" style="7"/>
     <col min="12296" max="12296" width="9" style="7" bestFit="1" customWidth="1"/>
     <col min="12297" max="12544" width="9" style="7"/>
-    <col min="12545" max="12545" width="11.3984375" style="7" customWidth="1"/>
-    <col min="12546" max="12546" width="9.59765625" style="7" bestFit="1" customWidth="1"/>
+    <col min="12545" max="12545" width="11.375" style="7" customWidth="1"/>
+    <col min="12546" max="12546" width="9.625" style="7" bestFit="1" customWidth="1"/>
     <col min="12547" max="12547" width="9" style="7" bestFit="1" customWidth="1"/>
-    <col min="12548" max="12549" width="8.59765625" style="7" bestFit="1" customWidth="1"/>
-    <col min="12550" max="12550" width="9.59765625" style="7" customWidth="1"/>
+    <col min="12548" max="12549" width="8.625" style="7" bestFit="1" customWidth="1"/>
+    <col min="12550" max="12550" width="9.625" style="7" customWidth="1"/>
     <col min="12551" max="12551" width="9" style="7"/>
     <col min="12552" max="12552" width="9" style="7" bestFit="1" customWidth="1"/>
     <col min="12553" max="12800" width="9" style="7"/>
-    <col min="12801" max="12801" width="11.3984375" style="7" customWidth="1"/>
-    <col min="12802" max="12802" width="9.59765625" style="7" bestFit="1" customWidth="1"/>
+    <col min="12801" max="12801" width="11.375" style="7" customWidth="1"/>
+    <col min="12802" max="12802" width="9.625" style="7" bestFit="1" customWidth="1"/>
     <col min="12803" max="12803" width="9" style="7" bestFit="1" customWidth="1"/>
-    <col min="12804" max="12805" width="8.59765625" style="7" bestFit="1" customWidth="1"/>
-    <col min="12806" max="12806" width="9.59765625" style="7" customWidth="1"/>
+    <col min="12804" max="12805" width="8.625" style="7" bestFit="1" customWidth="1"/>
+    <col min="12806" max="12806" width="9.625" style="7" customWidth="1"/>
     <col min="12807" max="12807" width="9" style="7"/>
     <col min="12808" max="12808" width="9" style="7" bestFit="1" customWidth="1"/>
     <col min="12809" max="13056" width="9" style="7"/>
-    <col min="13057" max="13057" width="11.3984375" style="7" customWidth="1"/>
-    <col min="13058" max="13058" width="9.59765625" style="7" bestFit="1" customWidth="1"/>
+    <col min="13057" max="13057" width="11.375" style="7" customWidth="1"/>
+    <col min="13058" max="13058" width="9.625" style="7" bestFit="1" customWidth="1"/>
     <col min="13059" max="13059" width="9" style="7" bestFit="1" customWidth="1"/>
-    <col min="13060" max="13061" width="8.59765625" style="7" bestFit="1" customWidth="1"/>
-    <col min="13062" max="13062" width="9.59765625" style="7" customWidth="1"/>
+    <col min="13060" max="13061" width="8.625" style="7" bestFit="1" customWidth="1"/>
+    <col min="13062" max="13062" width="9.625" style="7" customWidth="1"/>
     <col min="13063" max="13063" width="9" style="7"/>
     <col min="13064" max="13064" width="9" style="7" bestFit="1" customWidth="1"/>
     <col min="13065" max="13312" width="9" style="7"/>
-    <col min="13313" max="13313" width="11.3984375" style="7" customWidth="1"/>
-    <col min="13314" max="13314" width="9.59765625" style="7" bestFit="1" customWidth="1"/>
+    <col min="13313" max="13313" width="11.375" style="7" customWidth="1"/>
+    <col min="13314" max="13314" width="9.625" style="7" bestFit="1" customWidth="1"/>
     <col min="13315" max="13315" width="9" style="7" bestFit="1" customWidth="1"/>
-    <col min="13316" max="13317" width="8.59765625" style="7" bestFit="1" customWidth="1"/>
-    <col min="13318" max="13318" width="9.59765625" style="7" customWidth="1"/>
+    <col min="13316" max="13317" width="8.625" style="7" bestFit="1" customWidth="1"/>
+    <col min="13318" max="13318" width="9.625" style="7" customWidth="1"/>
     <col min="13319" max="13319" width="9" style="7"/>
     <col min="13320" max="13320" width="9" style="7" bestFit="1" customWidth="1"/>
     <col min="13321" max="13568" width="9" style="7"/>
-    <col min="13569" max="13569" width="11.3984375" style="7" customWidth="1"/>
-    <col min="13570" max="13570" width="9.59765625" style="7" bestFit="1" customWidth="1"/>
+    <col min="13569" max="13569" width="11.375" style="7" customWidth="1"/>
+    <col min="13570" max="13570" width="9.625" style="7" bestFit="1" customWidth="1"/>
     <col min="13571" max="13571" width="9" style="7" bestFit="1" customWidth="1"/>
-    <col min="13572" max="13573" width="8.59765625" style="7" bestFit="1" customWidth="1"/>
-    <col min="13574" max="13574" width="9.59765625" style="7" customWidth="1"/>
+    <col min="13572" max="13573" width="8.625" style="7" bestFit="1" customWidth="1"/>
+    <col min="13574" max="13574" width="9.625" style="7" customWidth="1"/>
     <col min="13575" max="13575" width="9" style="7"/>
     <col min="13576" max="13576" width="9" style="7" bestFit="1" customWidth="1"/>
     <col min="13577" max="13824" width="9" style="7"/>
-    <col min="13825" max="13825" width="11.3984375" style="7" customWidth="1"/>
-    <col min="13826" max="13826" width="9.59765625" style="7" bestFit="1" customWidth="1"/>
+    <col min="13825" max="13825" width="11.375" style="7" customWidth="1"/>
+    <col min="13826" max="13826" width="9.625" style="7" bestFit="1" customWidth="1"/>
     <col min="13827" max="13827" width="9" style="7" bestFit="1" customWidth="1"/>
-    <col min="13828" max="13829" width="8.59765625" style="7" bestFit="1" customWidth="1"/>
-    <col min="13830" max="13830" width="9.59765625" style="7" customWidth="1"/>
+    <col min="13828" max="13829" width="8.625" style="7" bestFit="1" customWidth="1"/>
+    <col min="13830" max="13830" width="9.625" style="7" customWidth="1"/>
     <col min="13831" max="13831" width="9" style="7"/>
     <col min="13832" max="13832" width="9" style="7" bestFit="1" customWidth="1"/>
     <col min="13833" max="14080" width="9" style="7"/>
-    <col min="14081" max="14081" width="11.3984375" style="7" customWidth="1"/>
-    <col min="14082" max="14082" width="9.59765625" style="7" bestFit="1" customWidth="1"/>
+    <col min="14081" max="14081" width="11.375" style="7" customWidth="1"/>
+    <col min="14082" max="14082" width="9.625" style="7" bestFit="1" customWidth="1"/>
     <col min="14083" max="14083" width="9" style="7" bestFit="1" customWidth="1"/>
-    <col min="14084" max="14085" width="8.59765625" style="7" bestFit="1" customWidth="1"/>
-    <col min="14086" max="14086" width="9.59765625" style="7" customWidth="1"/>
+    <col min="14084" max="14085" width="8.625" style="7" bestFit="1" customWidth="1"/>
+    <col min="14086" max="14086" width="9.625" style="7" customWidth="1"/>
     <col min="14087" max="14087" width="9" style="7"/>
     <col min="14088" max="14088" width="9" style="7" bestFit="1" customWidth="1"/>
     <col min="14089" max="14336" width="9" style="7"/>
-    <col min="14337" max="14337" width="11.3984375" style="7" customWidth="1"/>
-    <col min="14338" max="14338" width="9.59765625" style="7" bestFit="1" customWidth="1"/>
+    <col min="14337" max="14337" width="11.375" style="7" customWidth="1"/>
+    <col min="14338" max="14338" width="9.625" style="7" bestFit="1" customWidth="1"/>
     <col min="14339" max="14339" width="9" style="7" bestFit="1" customWidth="1"/>
-    <col min="14340" max="14341" width="8.59765625" style="7" bestFit="1" customWidth="1"/>
-    <col min="14342" max="14342" width="9.59765625" style="7" customWidth="1"/>
+    <col min="14340" max="14341" width="8.625" style="7" bestFit="1" customWidth="1"/>
+    <col min="14342" max="14342" width="9.625" style="7" customWidth="1"/>
     <col min="14343" max="14343" width="9" style="7"/>
     <col min="14344" max="14344" width="9" style="7" bestFit="1" customWidth="1"/>
     <col min="14345" max="14592" width="9" style="7"/>
-    <col min="14593" max="14593" width="11.3984375" style="7" customWidth="1"/>
-    <col min="14594" max="14594" width="9.59765625" style="7" bestFit="1" customWidth="1"/>
+    <col min="14593" max="14593" width="11.375" style="7" customWidth="1"/>
+    <col min="14594" max="14594" width="9.625" style="7" bestFit="1" customWidth="1"/>
     <col min="14595" max="14595" width="9" style="7" bestFit="1" customWidth="1"/>
-    <col min="14596" max="14597" width="8.59765625" style="7" bestFit="1" customWidth="1"/>
-    <col min="14598" max="14598" width="9.59765625" style="7" customWidth="1"/>
+    <col min="14596" max="14597" width="8.625" style="7" bestFit="1" customWidth="1"/>
+    <col min="14598" max="14598" width="9.625" style="7" customWidth="1"/>
     <col min="14599" max="14599" width="9" style="7"/>
     <col min="14600" max="14600" width="9" style="7" bestFit="1" customWidth="1"/>
     <col min="14601" max="14848" width="9" style="7"/>
-    <col min="14849" max="14849" width="11.3984375" style="7" customWidth="1"/>
-    <col min="14850" max="14850" width="9.59765625" style="7" bestFit="1" customWidth="1"/>
+    <col min="14849" max="14849" width="11.375" style="7" customWidth="1"/>
+    <col min="14850" max="14850" width="9.625" style="7" bestFit="1" customWidth="1"/>
     <col min="14851" max="14851" width="9" style="7" bestFit="1" customWidth="1"/>
-    <col min="14852" max="14853" width="8.59765625" style="7" bestFit="1" customWidth="1"/>
-    <col min="14854" max="14854" width="9.59765625" style="7" customWidth="1"/>
+    <col min="14852" max="14853" width="8.625" style="7" bestFit="1" customWidth="1"/>
+    <col min="14854" max="14854" width="9.625" style="7" customWidth="1"/>
     <col min="14855" max="14855" width="9" style="7"/>
     <col min="14856" max="14856" width="9" style="7" bestFit="1" customWidth="1"/>
     <col min="14857" max="15104" width="9" style="7"/>
-    <col min="15105" max="15105" width="11.3984375" style="7" customWidth="1"/>
-    <col min="15106" max="15106" width="9.59765625" style="7" bestFit="1" customWidth="1"/>
+    <col min="15105" max="15105" width="11.375" style="7" customWidth="1"/>
+    <col min="15106" max="15106" width="9.625" style="7" bestFit="1" customWidth="1"/>
     <col min="15107" max="15107" width="9" style="7" bestFit="1" customWidth="1"/>
-    <col min="15108" max="15109" width="8.59765625" style="7" bestFit="1" customWidth="1"/>
-    <col min="15110" max="15110" width="9.59765625" style="7" customWidth="1"/>
+    <col min="15108" max="15109" width="8.625" style="7" bestFit="1" customWidth="1"/>
+    <col min="15110" max="15110" width="9.625" style="7" customWidth="1"/>
     <col min="15111" max="15111" width="9" style="7"/>
     <col min="15112" max="15112" width="9" style="7" bestFit="1" customWidth="1"/>
     <col min="15113" max="15360" width="9" style="7"/>
-    <col min="15361" max="15361" width="11.3984375" style="7" customWidth="1"/>
-    <col min="15362" max="15362" width="9.59765625" style="7" bestFit="1" customWidth="1"/>
+    <col min="15361" max="15361" width="11.375" style="7" customWidth="1"/>
+    <col min="15362" max="15362" width="9.625" style="7" bestFit="1" customWidth="1"/>
     <col min="15363" max="15363" width="9" style="7" bestFit="1" customWidth="1"/>
-    <col min="15364" max="15365" width="8.59765625" style="7" bestFit="1" customWidth="1"/>
-    <col min="15366" max="15366" width="9.59765625" style="7" customWidth="1"/>
+    <col min="15364" max="15365" width="8.625" style="7" bestFit="1" customWidth="1"/>
+    <col min="15366" max="15366" width="9.625" style="7" customWidth="1"/>
     <col min="15367" max="15367" width="9" style="7"/>
     <col min="15368" max="15368" width="9" style="7" bestFit="1" customWidth="1"/>
     <col min="15369" max="15616" width="9" style="7"/>
-    <col min="15617" max="15617" width="11.3984375" style="7" customWidth="1"/>
-    <col min="15618" max="15618" width="9.59765625" style="7" bestFit="1" customWidth="1"/>
+    <col min="15617" max="15617" width="11.375" style="7" customWidth="1"/>
+    <col min="15618" max="15618" width="9.625" style="7" bestFit="1" customWidth="1"/>
     <col min="15619" max="15619" width="9" style="7" bestFit="1" customWidth="1"/>
-    <col min="15620" max="15621" width="8.59765625" style="7" bestFit="1" customWidth="1"/>
-    <col min="15622" max="15622" width="9.59765625" style="7" customWidth="1"/>
+    <col min="15620" max="15621" width="8.625" style="7" bestFit="1" customWidth="1"/>
+    <col min="15622" max="15622" width="9.625" style="7" customWidth="1"/>
     <col min="15623" max="15623" width="9" style="7"/>
     <col min="15624" max="15624" width="9" style="7" bestFit="1" customWidth="1"/>
     <col min="15625" max="15872" width="9" style="7"/>
-    <col min="15873" max="15873" width="11.3984375" style="7" customWidth="1"/>
-    <col min="15874" max="15874" width="9.59765625" style="7" bestFit="1" customWidth="1"/>
+    <col min="15873" max="15873" width="11.375" style="7" customWidth="1"/>
+    <col min="15874" max="15874" width="9.625" style="7" bestFit="1" customWidth="1"/>
     <col min="15875" max="15875" width="9" style="7" bestFit="1" customWidth="1"/>
-    <col min="15876" max="15877" width="8.59765625" style="7" bestFit="1" customWidth="1"/>
-    <col min="15878" max="15878" width="9.59765625" style="7" customWidth="1"/>
+    <col min="15876" max="15877" width="8.625" style="7" bestFit="1" customWidth="1"/>
+    <col min="15878" max="15878" width="9.625" style="7" customWidth="1"/>
     <col min="15879" max="15879" width="9" style="7"/>
     <col min="15880" max="15880" width="9" style="7" bestFit="1" customWidth="1"/>
     <col min="15881" max="16128" width="9" style="7"/>
-    <col min="16129" max="16129" width="11.3984375" style="7" customWidth="1"/>
-    <col min="16130" max="16130" width="9.59765625" style="7" bestFit="1" customWidth="1"/>
+    <col min="16129" max="16129" width="11.375" style="7" customWidth="1"/>
+    <col min="16130" max="16130" width="9.625" style="7" bestFit="1" customWidth="1"/>
     <col min="16131" max="16131" width="9" style="7" bestFit="1" customWidth="1"/>
-    <col min="16132" max="16133" width="8.59765625" style="7" bestFit="1" customWidth="1"/>
-    <col min="16134" max="16134" width="9.59765625" style="7" customWidth="1"/>
+    <col min="16132" max="16133" width="8.625" style="7" bestFit="1" customWidth="1"/>
+    <col min="16134" max="16134" width="9.625" style="7" customWidth="1"/>
     <col min="16135" max="16135" width="9" style="7"/>
     <col min="16136" max="16136" width="9" style="7" bestFit="1" customWidth="1"/>
     <col min="16137" max="16384" width="9" style="7"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" ht="50.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:8" ht="50.25" customHeight="1" x14ac:dyDescent="0.4">
       <c r="A1" s="1" t="s">
         <v>10</v>
       </c>
@@ -5888,7 +5840,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="2" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:8" ht="12.75" x14ac:dyDescent="0.35">
       <c r="A2" s="15">
         <v>44331</v>
       </c>
@@ -5912,7 +5864,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="3" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:8" ht="12.75" x14ac:dyDescent="0.35">
       <c r="A3" s="15">
         <v>44332</v>
       </c>
@@ -5936,7 +5888,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="4" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:8" ht="12.75" x14ac:dyDescent="0.35">
       <c r="A4" s="15">
         <v>44333</v>
       </c>
@@ -5960,7 +5912,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="5" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:8" ht="12.75" x14ac:dyDescent="0.35">
       <c r="A5" s="15">
         <v>44334</v>
       </c>
@@ -5984,7 +5936,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="6" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:8" ht="12.75" x14ac:dyDescent="0.35">
       <c r="A6" s="15">
         <v>44335</v>
       </c>
@@ -6008,7 +5960,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="7" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:8" ht="12.75" x14ac:dyDescent="0.35">
       <c r="A7" s="15">
         <v>44336</v>
       </c>
@@ -6032,7 +5984,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="8" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:8" ht="12.75" x14ac:dyDescent="0.35">
       <c r="A8" s="15">
         <v>44337</v>
       </c>
@@ -6056,7 +6008,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="9" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:8" ht="12.75" x14ac:dyDescent="0.35">
       <c r="A9" s="15">
         <v>44338</v>
       </c>
@@ -6080,7 +6032,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="10" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:8" ht="12.75" x14ac:dyDescent="0.35">
       <c r="A10" s="15">
         <v>44339</v>
       </c>
@@ -6104,7 +6056,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="11" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:8" ht="12.75" x14ac:dyDescent="0.35">
       <c r="A11" s="15">
         <v>44340</v>
       </c>
@@ -6128,7 +6080,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="12" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:8" ht="12.75" x14ac:dyDescent="0.35">
       <c r="A12" s="15">
         <v>44341</v>
       </c>
@@ -6152,7 +6104,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="13" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:8" ht="12.75" x14ac:dyDescent="0.35">
       <c r="A13" s="15">
         <v>44342</v>
       </c>
@@ -6176,7 +6128,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="14" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:8" ht="12.75" x14ac:dyDescent="0.35">
       <c r="A14" s="15">
         <v>44343</v>
       </c>
@@ -6200,7 +6152,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="15" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:8" ht="12.75" x14ac:dyDescent="0.35">
       <c r="A15" s="15">
         <v>44344</v>
       </c>
@@ -6224,7 +6176,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="16" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:8" ht="12.75" x14ac:dyDescent="0.35">
       <c r="A16" s="15">
         <v>44345</v>
       </c>
@@ -6248,7 +6200,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="17" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:8" ht="12.75" x14ac:dyDescent="0.35">
       <c r="A17" s="15">
         <v>44346</v>
       </c>
@@ -6272,7 +6224,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="18" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:8" ht="12.75" x14ac:dyDescent="0.35">
       <c r="A18" s="15">
         <v>44347</v>
       </c>
@@ -6296,7 +6248,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="19" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:8" ht="12.75" x14ac:dyDescent="0.35">
       <c r="A19" s="15">
         <v>44348</v>
       </c>
@@ -6320,7 +6272,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="20" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:8" ht="12.75" x14ac:dyDescent="0.35">
       <c r="A20" s="15">
         <v>44349</v>
       </c>
@@ -6344,7 +6296,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="21" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:8" ht="12.75" x14ac:dyDescent="0.35">
       <c r="A21" s="15">
         <v>44350</v>
       </c>
@@ -6368,7 +6320,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="22" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:8" ht="12.75" x14ac:dyDescent="0.35">
       <c r="A22" s="15">
         <v>44351</v>
       </c>
@@ -6392,7 +6344,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="23" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:8" ht="12.75" x14ac:dyDescent="0.35">
       <c r="A23" s="15">
         <v>44352</v>
       </c>
@@ -6416,7 +6368,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="24" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:8" ht="12.75" x14ac:dyDescent="0.35">
       <c r="A24" s="15">
         <v>44353</v>
       </c>
@@ -6440,7 +6392,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="25" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:8" ht="12.75" x14ac:dyDescent="0.35">
       <c r="A25" s="15">
         <v>44354</v>
       </c>
@@ -6464,7 +6416,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="26" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:8" ht="12.75" x14ac:dyDescent="0.35">
       <c r="A26" s="15">
         <v>44355</v>
       </c>
@@ -6488,7 +6440,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="27" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:8" ht="12.75" x14ac:dyDescent="0.35">
       <c r="A27" s="15">
         <v>44356</v>
       </c>
@@ -6512,7 +6464,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="28" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:8" ht="12.75" x14ac:dyDescent="0.35">
       <c r="A28" s="15">
         <v>44357</v>
       </c>
@@ -6536,7 +6488,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="29" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:8" ht="12.75" x14ac:dyDescent="0.35">
       <c r="A29" s="15">
         <v>44358</v>
       </c>
@@ -6560,7 +6512,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="30" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:8" ht="12.75" x14ac:dyDescent="0.35">
       <c r="A30" s="15">
         <v>44359</v>
       </c>
@@ -6584,7 +6536,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="31" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:8" ht="12.75" x14ac:dyDescent="0.35">
       <c r="A31" s="15">
         <v>44360</v>
       </c>
@@ -6608,7 +6560,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="32" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:8" ht="12.75" x14ac:dyDescent="0.35">
       <c r="A32" s="15">
         <v>44361</v>
       </c>
@@ -6632,7 +6584,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="33" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:8" ht="12.75" x14ac:dyDescent="0.35">
       <c r="A33" s="15">
         <v>44362</v>
       </c>
@@ -6656,7 +6608,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="34" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:8" ht="12.75" x14ac:dyDescent="0.35">
       <c r="A34" s="15">
         <v>44363</v>
       </c>
@@ -6680,7 +6632,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="35" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:8" ht="12.75" x14ac:dyDescent="0.35">
       <c r="A35" s="15">
         <v>44364</v>
       </c>
@@ -6704,7 +6656,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="36" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:8" ht="12.75" x14ac:dyDescent="0.35">
       <c r="A36" s="15">
         <v>44366</v>
       </c>
@@ -6728,7 +6680,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="37" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:8" ht="12.75" x14ac:dyDescent="0.35">
       <c r="A37" s="15">
         <v>44367</v>
       </c>
@@ -6752,7 +6704,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="38" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:8" ht="12.75" x14ac:dyDescent="0.35">
       <c r="A38" s="15">
         <v>44368</v>
       </c>
@@ -6776,7 +6728,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="39" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:8" ht="12.75" x14ac:dyDescent="0.35">
       <c r="A39" s="15">
         <v>44371</v>
       </c>
@@ -6800,7 +6752,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="40" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:8" ht="12.75" x14ac:dyDescent="0.35">
       <c r="A40" s="15">
         <v>44372</v>
       </c>
@@ -6824,7 +6776,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="41" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:8" ht="12.75" x14ac:dyDescent="0.35">
       <c r="A41" s="15">
         <v>44374</v>
       </c>
@@ -6848,7 +6800,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="42" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:8" ht="12.75" x14ac:dyDescent="0.35">
       <c r="A42" s="15">
         <v>44376</v>
       </c>
@@ -6872,7 +6824,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="43" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="43" spans="1:8" ht="12.75" x14ac:dyDescent="0.35">
       <c r="A43" s="15">
         <v>44379</v>
       </c>
@@ -6896,7 +6848,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="44" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="44" spans="1:8" ht="12.75" x14ac:dyDescent="0.35">
       <c r="A44" s="15">
         <v>44380</v>
       </c>
@@ -6920,7 +6872,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="45" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="45" spans="1:8" ht="12.75" x14ac:dyDescent="0.35">
       <c r="A45" s="15">
         <v>44381</v>
       </c>
@@ -6944,7 +6896,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="46" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="46" spans="1:8" ht="12.75" x14ac:dyDescent="0.35">
       <c r="A46" s="15">
         <v>44383</v>
       </c>
@@ -6968,7 +6920,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="47" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="47" spans="1:8" ht="12.75" x14ac:dyDescent="0.35">
       <c r="A47" s="15">
         <v>44384</v>
       </c>
@@ -6992,7 +6944,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="48" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="48" spans="1:8" ht="12.75" x14ac:dyDescent="0.35">
       <c r="A48" s="15">
         <v>44387</v>
       </c>
@@ -7016,7 +6968,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="49" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="49" spans="1:8" ht="12.75" x14ac:dyDescent="0.35">
       <c r="A49" s="15">
         <v>44388</v>
       </c>
@@ -7040,7 +6992,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="50" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="50" spans="1:8" ht="12.75" x14ac:dyDescent="0.35">
       <c r="A50" s="15">
         <v>44390</v>
       </c>
@@ -7064,7 +7016,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="51" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="51" spans="1:8" ht="12.75" x14ac:dyDescent="0.35">
       <c r="A51" s="15">
         <v>44392</v>
       </c>
@@ -7088,7 +7040,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="52" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="52" spans="1:8" ht="12.75" x14ac:dyDescent="0.35">
       <c r="A52" s="15">
         <v>44396</v>
       </c>
@@ -7112,7 +7064,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="53" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="53" spans="1:8" ht="12.75" x14ac:dyDescent="0.35">
       <c r="A53" s="15">
         <v>44397</v>
       </c>
@@ -7136,7 +7088,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="54" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="54" spans="1:8" ht="12.75" x14ac:dyDescent="0.35">
       <c r="A54" s="15">
         <v>44398</v>
       </c>
@@ -7160,7 +7112,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="55" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="55" spans="1:8" ht="12.75" x14ac:dyDescent="0.35">
       <c r="A55" s="15">
         <v>44399</v>
       </c>
@@ -7184,7 +7136,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="56" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="56" spans="1:8" ht="12.75" x14ac:dyDescent="0.35">
       <c r="A56" s="15">
         <v>44400</v>
       </c>
@@ -7208,7 +7160,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="57" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="57" spans="1:8" ht="12.75" x14ac:dyDescent="0.35">
       <c r="A57" s="15">
         <v>44401</v>
       </c>
@@ -7232,7 +7184,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="58" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="58" spans="1:8" ht="12.75" x14ac:dyDescent="0.35">
       <c r="A58" s="15">
         <v>44403</v>
       </c>
@@ -7256,7 +7208,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="59" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="59" spans="1:8" ht="12.75" x14ac:dyDescent="0.35">
       <c r="A59" s="15">
         <v>44404</v>
       </c>
@@ -7280,7 +7232,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="60" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="60" spans="1:8" ht="12.75" x14ac:dyDescent="0.35">
       <c r="A60" s="15">
         <v>44405</v>
       </c>
@@ -7304,7 +7256,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="61" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="61" spans="1:8" ht="12.75" x14ac:dyDescent="0.35">
       <c r="A61" s="15">
         <v>44406</v>
       </c>
@@ -7328,7 +7280,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="62" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="62" spans="1:8" ht="12.75" x14ac:dyDescent="0.35">
       <c r="A62" s="15">
         <v>44407</v>
       </c>
@@ -7352,7 +7304,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="63" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="63" spans="1:8" ht="12.75" x14ac:dyDescent="0.35">
       <c r="A63" s="15">
         <v>44408</v>
       </c>
@@ -7376,7 +7328,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="64" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="64" spans="1:8" x14ac:dyDescent="0.4">
       <c r="A64" s="8" t="s">
         <v>5</v>
       </c>
@@ -7439,8 +7391,7 @@
     <oddHeader>&amp;C&amp;"+,Bold"&amp;16&amp;A River Lottery Demand by Launch Date</oddHeader>
     <oddFooter>&amp;L&amp;A&amp;C&amp;"-,Bold"&amp;G USDA Forest Service&amp;RPage &amp;P of &amp;N</oddFooter>
   </headerFooter>
-  <legacyDrawing r:id="rId2"/>
-  <legacyDrawingHF r:id="rId3"/>
+  <legacyDrawingHF r:id="rId2"/>
 </worksheet>
 </file>
 
@@ -7454,523 +7405,523 @@
       <selection pane="bottomLeft" activeCell="L110" sqref="L110"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="13.2" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="13.15" x14ac:dyDescent="0.4"/>
   <cols>
-    <col min="1" max="1" width="13.09765625" style="11" customWidth="1"/>
-    <col min="2" max="2" width="9.59765625" style="12" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="13.125" style="11" customWidth="1"/>
+    <col min="2" max="2" width="9.625" style="12" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="9" style="12" bestFit="1" customWidth="1"/>
-    <col min="4" max="5" width="8.59765625" style="12" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="9.59765625" style="10" customWidth="1"/>
-    <col min="7" max="7" width="3.59765625" style="7" customWidth="1"/>
+    <col min="4" max="5" width="8.625" style="12" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="9.625" style="10" customWidth="1"/>
+    <col min="7" max="7" width="3.625" style="7" customWidth="1"/>
     <col min="8" max="8" width="9" style="12" bestFit="1" customWidth="1"/>
     <col min="9" max="256" width="9" style="7"/>
-    <col min="257" max="257" width="11.3984375" style="7" customWidth="1"/>
-    <col min="258" max="258" width="9.59765625" style="7" bestFit="1" customWidth="1"/>
+    <col min="257" max="257" width="11.375" style="7" customWidth="1"/>
+    <col min="258" max="258" width="9.625" style="7" bestFit="1" customWidth="1"/>
     <col min="259" max="259" width="9" style="7" bestFit="1" customWidth="1"/>
-    <col min="260" max="261" width="8.59765625" style="7" bestFit="1" customWidth="1"/>
-    <col min="262" max="262" width="9.59765625" style="7" customWidth="1"/>
+    <col min="260" max="261" width="8.625" style="7" bestFit="1" customWidth="1"/>
+    <col min="262" max="262" width="9.625" style="7" customWidth="1"/>
     <col min="263" max="263" width="9" style="7"/>
     <col min="264" max="264" width="9" style="7" bestFit="1" customWidth="1"/>
     <col min="265" max="512" width="9" style="7"/>
-    <col min="513" max="513" width="11.3984375" style="7" customWidth="1"/>
-    <col min="514" max="514" width="9.59765625" style="7" bestFit="1" customWidth="1"/>
+    <col min="513" max="513" width="11.375" style="7" customWidth="1"/>
+    <col min="514" max="514" width="9.625" style="7" bestFit="1" customWidth="1"/>
     <col min="515" max="515" width="9" style="7" bestFit="1" customWidth="1"/>
-    <col min="516" max="517" width="8.59765625" style="7" bestFit="1" customWidth="1"/>
-    <col min="518" max="518" width="9.59765625" style="7" customWidth="1"/>
+    <col min="516" max="517" width="8.625" style="7" bestFit="1" customWidth="1"/>
+    <col min="518" max="518" width="9.625" style="7" customWidth="1"/>
     <col min="519" max="519" width="9" style="7"/>
     <col min="520" max="520" width="9" style="7" bestFit="1" customWidth="1"/>
     <col min="521" max="768" width="9" style="7"/>
-    <col min="769" max="769" width="11.3984375" style="7" customWidth="1"/>
-    <col min="770" max="770" width="9.59765625" style="7" bestFit="1" customWidth="1"/>
+    <col min="769" max="769" width="11.375" style="7" customWidth="1"/>
+    <col min="770" max="770" width="9.625" style="7" bestFit="1" customWidth="1"/>
     <col min="771" max="771" width="9" style="7" bestFit="1" customWidth="1"/>
-    <col min="772" max="773" width="8.59765625" style="7" bestFit="1" customWidth="1"/>
-    <col min="774" max="774" width="9.59765625" style="7" customWidth="1"/>
+    <col min="772" max="773" width="8.625" style="7" bestFit="1" customWidth="1"/>
+    <col min="774" max="774" width="9.625" style="7" customWidth="1"/>
     <col min="775" max="775" width="9" style="7"/>
     <col min="776" max="776" width="9" style="7" bestFit="1" customWidth="1"/>
     <col min="777" max="1024" width="9" style="7"/>
-    <col min="1025" max="1025" width="11.3984375" style="7" customWidth="1"/>
-    <col min="1026" max="1026" width="9.59765625" style="7" bestFit="1" customWidth="1"/>
+    <col min="1025" max="1025" width="11.375" style="7" customWidth="1"/>
+    <col min="1026" max="1026" width="9.625" style="7" bestFit="1" customWidth="1"/>
     <col min="1027" max="1027" width="9" style="7" bestFit="1" customWidth="1"/>
-    <col min="1028" max="1029" width="8.59765625" style="7" bestFit="1" customWidth="1"/>
-    <col min="1030" max="1030" width="9.59765625" style="7" customWidth="1"/>
+    <col min="1028" max="1029" width="8.625" style="7" bestFit="1" customWidth="1"/>
+    <col min="1030" max="1030" width="9.625" style="7" customWidth="1"/>
     <col min="1031" max="1031" width="9" style="7"/>
     <col min="1032" max="1032" width="9" style="7" bestFit="1" customWidth="1"/>
     <col min="1033" max="1280" width="9" style="7"/>
-    <col min="1281" max="1281" width="11.3984375" style="7" customWidth="1"/>
-    <col min="1282" max="1282" width="9.59765625" style="7" bestFit="1" customWidth="1"/>
+    <col min="1281" max="1281" width="11.375" style="7" customWidth="1"/>
+    <col min="1282" max="1282" width="9.625" style="7" bestFit="1" customWidth="1"/>
     <col min="1283" max="1283" width="9" style="7" bestFit="1" customWidth="1"/>
-    <col min="1284" max="1285" width="8.59765625" style="7" bestFit="1" customWidth="1"/>
-    <col min="1286" max="1286" width="9.59765625" style="7" customWidth="1"/>
+    <col min="1284" max="1285" width="8.625" style="7" bestFit="1" customWidth="1"/>
+    <col min="1286" max="1286" width="9.625" style="7" customWidth="1"/>
     <col min="1287" max="1287" width="9" style="7"/>
     <col min="1288" max="1288" width="9" style="7" bestFit="1" customWidth="1"/>
     <col min="1289" max="1536" width="9" style="7"/>
-    <col min="1537" max="1537" width="11.3984375" style="7" customWidth="1"/>
-    <col min="1538" max="1538" width="9.59765625" style="7" bestFit="1" customWidth="1"/>
+    <col min="1537" max="1537" width="11.375" style="7" customWidth="1"/>
+    <col min="1538" max="1538" width="9.625" style="7" bestFit="1" customWidth="1"/>
     <col min="1539" max="1539" width="9" style="7" bestFit="1" customWidth="1"/>
-    <col min="1540" max="1541" width="8.59765625" style="7" bestFit="1" customWidth="1"/>
-    <col min="1542" max="1542" width="9.59765625" style="7" customWidth="1"/>
+    <col min="1540" max="1541" width="8.625" style="7" bestFit="1" customWidth="1"/>
+    <col min="1542" max="1542" width="9.625" style="7" customWidth="1"/>
     <col min="1543" max="1543" width="9" style="7"/>
     <col min="1544" max="1544" width="9" style="7" bestFit="1" customWidth="1"/>
     <col min="1545" max="1792" width="9" style="7"/>
-    <col min="1793" max="1793" width="11.3984375" style="7" customWidth="1"/>
-    <col min="1794" max="1794" width="9.59765625" style="7" bestFit="1" customWidth="1"/>
+    <col min="1793" max="1793" width="11.375" style="7" customWidth="1"/>
+    <col min="1794" max="1794" width="9.625" style="7" bestFit="1" customWidth="1"/>
     <col min="1795" max="1795" width="9" style="7" bestFit="1" customWidth="1"/>
-    <col min="1796" max="1797" width="8.59765625" style="7" bestFit="1" customWidth="1"/>
-    <col min="1798" max="1798" width="9.59765625" style="7" customWidth="1"/>
+    <col min="1796" max="1797" width="8.625" style="7" bestFit="1" customWidth="1"/>
+    <col min="1798" max="1798" width="9.625" style="7" customWidth="1"/>
     <col min="1799" max="1799" width="9" style="7"/>
     <col min="1800" max="1800" width="9" style="7" bestFit="1" customWidth="1"/>
     <col min="1801" max="2048" width="9" style="7"/>
-    <col min="2049" max="2049" width="11.3984375" style="7" customWidth="1"/>
-    <col min="2050" max="2050" width="9.59765625" style="7" bestFit="1" customWidth="1"/>
+    <col min="2049" max="2049" width="11.375" style="7" customWidth="1"/>
+    <col min="2050" max="2050" width="9.625" style="7" bestFit="1" customWidth="1"/>
     <col min="2051" max="2051" width="9" style="7" bestFit="1" customWidth="1"/>
-    <col min="2052" max="2053" width="8.59765625" style="7" bestFit="1" customWidth="1"/>
-    <col min="2054" max="2054" width="9.59765625" style="7" customWidth="1"/>
+    <col min="2052" max="2053" width="8.625" style="7" bestFit="1" customWidth="1"/>
+    <col min="2054" max="2054" width="9.625" style="7" customWidth="1"/>
     <col min="2055" max="2055" width="9" style="7"/>
     <col min="2056" max="2056" width="9" style="7" bestFit="1" customWidth="1"/>
     <col min="2057" max="2304" width="9" style="7"/>
-    <col min="2305" max="2305" width="11.3984375" style="7" customWidth="1"/>
-    <col min="2306" max="2306" width="9.59765625" style="7" bestFit="1" customWidth="1"/>
+    <col min="2305" max="2305" width="11.375" style="7" customWidth="1"/>
+    <col min="2306" max="2306" width="9.625" style="7" bestFit="1" customWidth="1"/>
     <col min="2307" max="2307" width="9" style="7" bestFit="1" customWidth="1"/>
-    <col min="2308" max="2309" width="8.59765625" style="7" bestFit="1" customWidth="1"/>
-    <col min="2310" max="2310" width="9.59765625" style="7" customWidth="1"/>
+    <col min="2308" max="2309" width="8.625" style="7" bestFit="1" customWidth="1"/>
+    <col min="2310" max="2310" width="9.625" style="7" customWidth="1"/>
     <col min="2311" max="2311" width="9" style="7"/>
     <col min="2312" max="2312" width="9" style="7" bestFit="1" customWidth="1"/>
     <col min="2313" max="2560" width="9" style="7"/>
-    <col min="2561" max="2561" width="11.3984375" style="7" customWidth="1"/>
-    <col min="2562" max="2562" width="9.59765625" style="7" bestFit="1" customWidth="1"/>
+    <col min="2561" max="2561" width="11.375" style="7" customWidth="1"/>
+    <col min="2562" max="2562" width="9.625" style="7" bestFit="1" customWidth="1"/>
     <col min="2563" max="2563" width="9" style="7" bestFit="1" customWidth="1"/>
-    <col min="2564" max="2565" width="8.59765625" style="7" bestFit="1" customWidth="1"/>
-    <col min="2566" max="2566" width="9.59765625" style="7" customWidth="1"/>
+    <col min="2564" max="2565" width="8.625" style="7" bestFit="1" customWidth="1"/>
+    <col min="2566" max="2566" width="9.625" style="7" customWidth="1"/>
     <col min="2567" max="2567" width="9" style="7"/>
     <col min="2568" max="2568" width="9" style="7" bestFit="1" customWidth="1"/>
     <col min="2569" max="2816" width="9" style="7"/>
-    <col min="2817" max="2817" width="11.3984375" style="7" customWidth="1"/>
-    <col min="2818" max="2818" width="9.59765625" style="7" bestFit="1" customWidth="1"/>
+    <col min="2817" max="2817" width="11.375" style="7" customWidth="1"/>
+    <col min="2818" max="2818" width="9.625" style="7" bestFit="1" customWidth="1"/>
     <col min="2819" max="2819" width="9" style="7" bestFit="1" customWidth="1"/>
-    <col min="2820" max="2821" width="8.59765625" style="7" bestFit="1" customWidth="1"/>
-    <col min="2822" max="2822" width="9.59765625" style="7" customWidth="1"/>
+    <col min="2820" max="2821" width="8.625" style="7" bestFit="1" customWidth="1"/>
+    <col min="2822" max="2822" width="9.625" style="7" customWidth="1"/>
     <col min="2823" max="2823" width="9" style="7"/>
     <col min="2824" max="2824" width="9" style="7" bestFit="1" customWidth="1"/>
     <col min="2825" max="3072" width="9" style="7"/>
-    <col min="3073" max="3073" width="11.3984375" style="7" customWidth="1"/>
-    <col min="3074" max="3074" width="9.59765625" style="7" bestFit="1" customWidth="1"/>
+    <col min="3073" max="3073" width="11.375" style="7" customWidth="1"/>
+    <col min="3074" max="3074" width="9.625" style="7" bestFit="1" customWidth="1"/>
     <col min="3075" max="3075" width="9" style="7" bestFit="1" customWidth="1"/>
-    <col min="3076" max="3077" width="8.59765625" style="7" bestFit="1" customWidth="1"/>
-    <col min="3078" max="3078" width="9.59765625" style="7" customWidth="1"/>
+    <col min="3076" max="3077" width="8.625" style="7" bestFit="1" customWidth="1"/>
+    <col min="3078" max="3078" width="9.625" style="7" customWidth="1"/>
     <col min="3079" max="3079" width="9" style="7"/>
     <col min="3080" max="3080" width="9" style="7" bestFit="1" customWidth="1"/>
     <col min="3081" max="3328" width="9" style="7"/>
-    <col min="3329" max="3329" width="11.3984375" style="7" customWidth="1"/>
-    <col min="3330" max="3330" width="9.59765625" style="7" bestFit="1" customWidth="1"/>
+    <col min="3329" max="3329" width="11.375" style="7" customWidth="1"/>
+    <col min="3330" max="3330" width="9.625" style="7" bestFit="1" customWidth="1"/>
     <col min="3331" max="3331" width="9" style="7" bestFit="1" customWidth="1"/>
-    <col min="3332" max="3333" width="8.59765625" style="7" bestFit="1" customWidth="1"/>
-    <col min="3334" max="3334" width="9.59765625" style="7" customWidth="1"/>
+    <col min="3332" max="3333" width="8.625" style="7" bestFit="1" customWidth="1"/>
+    <col min="3334" max="3334" width="9.625" style="7" customWidth="1"/>
     <col min="3335" max="3335" width="9" style="7"/>
     <col min="3336" max="3336" width="9" style="7" bestFit="1" customWidth="1"/>
     <col min="3337" max="3584" width="9" style="7"/>
-    <col min="3585" max="3585" width="11.3984375" style="7" customWidth="1"/>
-    <col min="3586" max="3586" width="9.59765625" style="7" bestFit="1" customWidth="1"/>
+    <col min="3585" max="3585" width="11.375" style="7" customWidth="1"/>
+    <col min="3586" max="3586" width="9.625" style="7" bestFit="1" customWidth="1"/>
     <col min="3587" max="3587" width="9" style="7" bestFit="1" customWidth="1"/>
-    <col min="3588" max="3589" width="8.59765625" style="7" bestFit="1" customWidth="1"/>
-    <col min="3590" max="3590" width="9.59765625" style="7" customWidth="1"/>
+    <col min="3588" max="3589" width="8.625" style="7" bestFit="1" customWidth="1"/>
+    <col min="3590" max="3590" width="9.625" style="7" customWidth="1"/>
     <col min="3591" max="3591" width="9" style="7"/>
     <col min="3592" max="3592" width="9" style="7" bestFit="1" customWidth="1"/>
     <col min="3593" max="3840" width="9" style="7"/>
-    <col min="3841" max="3841" width="11.3984375" style="7" customWidth="1"/>
-    <col min="3842" max="3842" width="9.59765625" style="7" bestFit="1" customWidth="1"/>
+    <col min="3841" max="3841" width="11.375" style="7" customWidth="1"/>
+    <col min="3842" max="3842" width="9.625" style="7" bestFit="1" customWidth="1"/>
     <col min="3843" max="3843" width="9" style="7" bestFit="1" customWidth="1"/>
-    <col min="3844" max="3845" width="8.59765625" style="7" bestFit="1" customWidth="1"/>
-    <col min="3846" max="3846" width="9.59765625" style="7" customWidth="1"/>
+    <col min="3844" max="3845" width="8.625" style="7" bestFit="1" customWidth="1"/>
+    <col min="3846" max="3846" width="9.625" style="7" customWidth="1"/>
     <col min="3847" max="3847" width="9" style="7"/>
     <col min="3848" max="3848" width="9" style="7" bestFit="1" customWidth="1"/>
     <col min="3849" max="4096" width="9" style="7"/>
-    <col min="4097" max="4097" width="11.3984375" style="7" customWidth="1"/>
-    <col min="4098" max="4098" width="9.59765625" style="7" bestFit="1" customWidth="1"/>
+    <col min="4097" max="4097" width="11.375" style="7" customWidth="1"/>
+    <col min="4098" max="4098" width="9.625" style="7" bestFit="1" customWidth="1"/>
     <col min="4099" max="4099" width="9" style="7" bestFit="1" customWidth="1"/>
-    <col min="4100" max="4101" width="8.59765625" style="7" bestFit="1" customWidth="1"/>
-    <col min="4102" max="4102" width="9.59765625" style="7" customWidth="1"/>
+    <col min="4100" max="4101" width="8.625" style="7" bestFit="1" customWidth="1"/>
+    <col min="4102" max="4102" width="9.625" style="7" customWidth="1"/>
     <col min="4103" max="4103" width="9" style="7"/>
     <col min="4104" max="4104" width="9" style="7" bestFit="1" customWidth="1"/>
     <col min="4105" max="4352" width="9" style="7"/>
-    <col min="4353" max="4353" width="11.3984375" style="7" customWidth="1"/>
-    <col min="4354" max="4354" width="9.59765625" style="7" bestFit="1" customWidth="1"/>
+    <col min="4353" max="4353" width="11.375" style="7" customWidth="1"/>
+    <col min="4354" max="4354" width="9.625" style="7" bestFit="1" customWidth="1"/>
     <col min="4355" max="4355" width="9" style="7" bestFit="1" customWidth="1"/>
-    <col min="4356" max="4357" width="8.59765625" style="7" bestFit="1" customWidth="1"/>
-    <col min="4358" max="4358" width="9.59765625" style="7" customWidth="1"/>
+    <col min="4356" max="4357" width="8.625" style="7" bestFit="1" customWidth="1"/>
+    <col min="4358" max="4358" width="9.625" style="7" customWidth="1"/>
     <col min="4359" max="4359" width="9" style="7"/>
     <col min="4360" max="4360" width="9" style="7" bestFit="1" customWidth="1"/>
     <col min="4361" max="4608" width="9" style="7"/>
-    <col min="4609" max="4609" width="11.3984375" style="7" customWidth="1"/>
-    <col min="4610" max="4610" width="9.59765625" style="7" bestFit="1" customWidth="1"/>
+    <col min="4609" max="4609" width="11.375" style="7" customWidth="1"/>
+    <col min="4610" max="4610" width="9.625" style="7" bestFit="1" customWidth="1"/>
     <col min="4611" max="4611" width="9" style="7" bestFit="1" customWidth="1"/>
-    <col min="4612" max="4613" width="8.59765625" style="7" bestFit="1" customWidth="1"/>
-    <col min="4614" max="4614" width="9.59765625" style="7" customWidth="1"/>
+    <col min="4612" max="4613" width="8.625" style="7" bestFit="1" customWidth="1"/>
+    <col min="4614" max="4614" width="9.625" style="7" customWidth="1"/>
     <col min="4615" max="4615" width="9" style="7"/>
     <col min="4616" max="4616" width="9" style="7" bestFit="1" customWidth="1"/>
     <col min="4617" max="4864" width="9" style="7"/>
-    <col min="4865" max="4865" width="11.3984375" style="7" customWidth="1"/>
-    <col min="4866" max="4866" width="9.59765625" style="7" bestFit="1" customWidth="1"/>
+    <col min="4865" max="4865" width="11.375" style="7" customWidth="1"/>
+    <col min="4866" max="4866" width="9.625" style="7" bestFit="1" customWidth="1"/>
     <col min="4867" max="4867" width="9" style="7" bestFit="1" customWidth="1"/>
-    <col min="4868" max="4869" width="8.59765625" style="7" bestFit="1" customWidth="1"/>
-    <col min="4870" max="4870" width="9.59765625" style="7" customWidth="1"/>
+    <col min="4868" max="4869" width="8.625" style="7" bestFit="1" customWidth="1"/>
+    <col min="4870" max="4870" width="9.625" style="7" customWidth="1"/>
     <col min="4871" max="4871" width="9" style="7"/>
     <col min="4872" max="4872" width="9" style="7" bestFit="1" customWidth="1"/>
     <col min="4873" max="5120" width="9" style="7"/>
-    <col min="5121" max="5121" width="11.3984375" style="7" customWidth="1"/>
-    <col min="5122" max="5122" width="9.59765625" style="7" bestFit="1" customWidth="1"/>
+    <col min="5121" max="5121" width="11.375" style="7" customWidth="1"/>
+    <col min="5122" max="5122" width="9.625" style="7" bestFit="1" customWidth="1"/>
     <col min="5123" max="5123" width="9" style="7" bestFit="1" customWidth="1"/>
-    <col min="5124" max="5125" width="8.59765625" style="7" bestFit="1" customWidth="1"/>
-    <col min="5126" max="5126" width="9.59765625" style="7" customWidth="1"/>
+    <col min="5124" max="5125" width="8.625" style="7" bestFit="1" customWidth="1"/>
+    <col min="5126" max="5126" width="9.625" style="7" customWidth="1"/>
     <col min="5127" max="5127" width="9" style="7"/>
     <col min="5128" max="5128" width="9" style="7" bestFit="1" customWidth="1"/>
     <col min="5129" max="5376" width="9" style="7"/>
-    <col min="5377" max="5377" width="11.3984375" style="7" customWidth="1"/>
-    <col min="5378" max="5378" width="9.59765625" style="7" bestFit="1" customWidth="1"/>
+    <col min="5377" max="5377" width="11.375" style="7" customWidth="1"/>
+    <col min="5378" max="5378" width="9.625" style="7" bestFit="1" customWidth="1"/>
     <col min="5379" max="5379" width="9" style="7" bestFit="1" customWidth="1"/>
-    <col min="5380" max="5381" width="8.59765625" style="7" bestFit="1" customWidth="1"/>
-    <col min="5382" max="5382" width="9.59765625" style="7" customWidth="1"/>
+    <col min="5380" max="5381" width="8.625" style="7" bestFit="1" customWidth="1"/>
+    <col min="5382" max="5382" width="9.625" style="7" customWidth="1"/>
     <col min="5383" max="5383" width="9" style="7"/>
     <col min="5384" max="5384" width="9" style="7" bestFit="1" customWidth="1"/>
     <col min="5385" max="5632" width="9" style="7"/>
-    <col min="5633" max="5633" width="11.3984375" style="7" customWidth="1"/>
-    <col min="5634" max="5634" width="9.59765625" style="7" bestFit="1" customWidth="1"/>
+    <col min="5633" max="5633" width="11.375" style="7" customWidth="1"/>
+    <col min="5634" max="5634" width="9.625" style="7" bestFit="1" customWidth="1"/>
     <col min="5635" max="5635" width="9" style="7" bestFit="1" customWidth="1"/>
-    <col min="5636" max="5637" width="8.59765625" style="7" bestFit="1" customWidth="1"/>
-    <col min="5638" max="5638" width="9.59765625" style="7" customWidth="1"/>
+    <col min="5636" max="5637" width="8.625" style="7" bestFit="1" customWidth="1"/>
+    <col min="5638" max="5638" width="9.625" style="7" customWidth="1"/>
     <col min="5639" max="5639" width="9" style="7"/>
     <col min="5640" max="5640" width="9" style="7" bestFit="1" customWidth="1"/>
     <col min="5641" max="5888" width="9" style="7"/>
-    <col min="5889" max="5889" width="11.3984375" style="7" customWidth="1"/>
-    <col min="5890" max="5890" width="9.59765625" style="7" bestFit="1" customWidth="1"/>
+    <col min="5889" max="5889" width="11.375" style="7" customWidth="1"/>
+    <col min="5890" max="5890" width="9.625" style="7" bestFit="1" customWidth="1"/>
     <col min="5891" max="5891" width="9" style="7" bestFit="1" customWidth="1"/>
-    <col min="5892" max="5893" width="8.59765625" style="7" bestFit="1" customWidth="1"/>
-    <col min="5894" max="5894" width="9.59765625" style="7" customWidth="1"/>
+    <col min="5892" max="5893" width="8.625" style="7" bestFit="1" customWidth="1"/>
+    <col min="5894" max="5894" width="9.625" style="7" customWidth="1"/>
     <col min="5895" max="5895" width="9" style="7"/>
     <col min="5896" max="5896" width="9" style="7" bestFit="1" customWidth="1"/>
     <col min="5897" max="6144" width="9" style="7"/>
-    <col min="6145" max="6145" width="11.3984375" style="7" customWidth="1"/>
-    <col min="6146" max="6146" width="9.59765625" style="7" bestFit="1" customWidth="1"/>
+    <col min="6145" max="6145" width="11.375" style="7" customWidth="1"/>
+    <col min="6146" max="6146" width="9.625" style="7" bestFit="1" customWidth="1"/>
     <col min="6147" max="6147" width="9" style="7" bestFit="1" customWidth="1"/>
-    <col min="6148" max="6149" width="8.59765625" style="7" bestFit="1" customWidth="1"/>
-    <col min="6150" max="6150" width="9.59765625" style="7" customWidth="1"/>
+    <col min="6148" max="6149" width="8.625" style="7" bestFit="1" customWidth="1"/>
+    <col min="6150" max="6150" width="9.625" style="7" customWidth="1"/>
     <col min="6151" max="6151" width="9" style="7"/>
     <col min="6152" max="6152" width="9" style="7" bestFit="1" customWidth="1"/>
     <col min="6153" max="6400" width="9" style="7"/>
-    <col min="6401" max="6401" width="11.3984375" style="7" customWidth="1"/>
-    <col min="6402" max="6402" width="9.59765625" style="7" bestFit="1" customWidth="1"/>
+    <col min="6401" max="6401" width="11.375" style="7" customWidth="1"/>
+    <col min="6402" max="6402" width="9.625" style="7" bestFit="1" customWidth="1"/>
     <col min="6403" max="6403" width="9" style="7" bestFit="1" customWidth="1"/>
-    <col min="6404" max="6405" width="8.59765625" style="7" bestFit="1" customWidth="1"/>
-    <col min="6406" max="6406" width="9.59765625" style="7" customWidth="1"/>
+    <col min="6404" max="6405" width="8.625" style="7" bestFit="1" customWidth="1"/>
+    <col min="6406" max="6406" width="9.625" style="7" customWidth="1"/>
     <col min="6407" max="6407" width="9" style="7"/>
     <col min="6408" max="6408" width="9" style="7" bestFit="1" customWidth="1"/>
     <col min="6409" max="6656" width="9" style="7"/>
-    <col min="6657" max="6657" width="11.3984375" style="7" customWidth="1"/>
-    <col min="6658" max="6658" width="9.59765625" style="7" bestFit="1" customWidth="1"/>
+    <col min="6657" max="6657" width="11.375" style="7" customWidth="1"/>
+    <col min="6658" max="6658" width="9.625" style="7" bestFit="1" customWidth="1"/>
     <col min="6659" max="6659" width="9" style="7" bestFit="1" customWidth="1"/>
-    <col min="6660" max="6661" width="8.59765625" style="7" bestFit="1" customWidth="1"/>
-    <col min="6662" max="6662" width="9.59765625" style="7" customWidth="1"/>
+    <col min="6660" max="6661" width="8.625" style="7" bestFit="1" customWidth="1"/>
+    <col min="6662" max="6662" width="9.625" style="7" customWidth="1"/>
     <col min="6663" max="6663" width="9" style="7"/>
     <col min="6664" max="6664" width="9" style="7" bestFit="1" customWidth="1"/>
     <col min="6665" max="6912" width="9" style="7"/>
-    <col min="6913" max="6913" width="11.3984375" style="7" customWidth="1"/>
-    <col min="6914" max="6914" width="9.59765625" style="7" bestFit="1" customWidth="1"/>
+    <col min="6913" max="6913" width="11.375" style="7" customWidth="1"/>
+    <col min="6914" max="6914" width="9.625" style="7" bestFit="1" customWidth="1"/>
     <col min="6915" max="6915" width="9" style="7" bestFit="1" customWidth="1"/>
-    <col min="6916" max="6917" width="8.59765625" style="7" bestFit="1" customWidth="1"/>
-    <col min="6918" max="6918" width="9.59765625" style="7" customWidth="1"/>
+    <col min="6916" max="6917" width="8.625" style="7" bestFit="1" customWidth="1"/>
+    <col min="6918" max="6918" width="9.625" style="7" customWidth="1"/>
     <col min="6919" max="6919" width="9" style="7"/>
     <col min="6920" max="6920" width="9" style="7" bestFit="1" customWidth="1"/>
     <col min="6921" max="7168" width="9" style="7"/>
-    <col min="7169" max="7169" width="11.3984375" style="7" customWidth="1"/>
-    <col min="7170" max="7170" width="9.59765625" style="7" bestFit="1" customWidth="1"/>
+    <col min="7169" max="7169" width="11.375" style="7" customWidth="1"/>
+    <col min="7170" max="7170" width="9.625" style="7" bestFit="1" customWidth="1"/>
     <col min="7171" max="7171" width="9" style="7" bestFit="1" customWidth="1"/>
-    <col min="7172" max="7173" width="8.59765625" style="7" bestFit="1" customWidth="1"/>
-    <col min="7174" max="7174" width="9.59765625" style="7" customWidth="1"/>
+    <col min="7172" max="7173" width="8.625" style="7" bestFit="1" customWidth="1"/>
+    <col min="7174" max="7174" width="9.625" style="7" customWidth="1"/>
     <col min="7175" max="7175" width="9" style="7"/>
     <col min="7176" max="7176" width="9" style="7" bestFit="1" customWidth="1"/>
     <col min="7177" max="7424" width="9" style="7"/>
-    <col min="7425" max="7425" width="11.3984375" style="7" customWidth="1"/>
-    <col min="7426" max="7426" width="9.59765625" style="7" bestFit="1" customWidth="1"/>
+    <col min="7425" max="7425" width="11.375" style="7" customWidth="1"/>
+    <col min="7426" max="7426" width="9.625" style="7" bestFit="1" customWidth="1"/>
     <col min="7427" max="7427" width="9" style="7" bestFit="1" customWidth="1"/>
-    <col min="7428" max="7429" width="8.59765625" style="7" bestFit="1" customWidth="1"/>
-    <col min="7430" max="7430" width="9.59765625" style="7" customWidth="1"/>
+    <col min="7428" max="7429" width="8.625" style="7" bestFit="1" customWidth="1"/>
+    <col min="7430" max="7430" width="9.625" style="7" customWidth="1"/>
     <col min="7431" max="7431" width="9" style="7"/>
     <col min="7432" max="7432" width="9" style="7" bestFit="1" customWidth="1"/>
     <col min="7433" max="7680" width="9" style="7"/>
-    <col min="7681" max="7681" width="11.3984375" style="7" customWidth="1"/>
-    <col min="7682" max="7682" width="9.59765625" style="7" bestFit="1" customWidth="1"/>
+    <col min="7681" max="7681" width="11.375" style="7" customWidth="1"/>
+    <col min="7682" max="7682" width="9.625" style="7" bestFit="1" customWidth="1"/>
     <col min="7683" max="7683" width="9" style="7" bestFit="1" customWidth="1"/>
-    <col min="7684" max="7685" width="8.59765625" style="7" bestFit="1" customWidth="1"/>
-    <col min="7686" max="7686" width="9.59765625" style="7" customWidth="1"/>
+    <col min="7684" max="7685" width="8.625" style="7" bestFit="1" customWidth="1"/>
+    <col min="7686" max="7686" width="9.625" style="7" customWidth="1"/>
     <col min="7687" max="7687" width="9" style="7"/>
     <col min="7688" max="7688" width="9" style="7" bestFit="1" customWidth="1"/>
     <col min="7689" max="7936" width="9" style="7"/>
-    <col min="7937" max="7937" width="11.3984375" style="7" customWidth="1"/>
-    <col min="7938" max="7938" width="9.59765625" style="7" bestFit="1" customWidth="1"/>
+    <col min="7937" max="7937" width="11.375" style="7" customWidth="1"/>
+    <col min="7938" max="7938" width="9.625" style="7" bestFit="1" customWidth="1"/>
     <col min="7939" max="7939" width="9" style="7" bestFit="1" customWidth="1"/>
-    <col min="7940" max="7941" width="8.59765625" style="7" bestFit="1" customWidth="1"/>
-    <col min="7942" max="7942" width="9.59765625" style="7" customWidth="1"/>
+    <col min="7940" max="7941" width="8.625" style="7" bestFit="1" customWidth="1"/>
+    <col min="7942" max="7942" width="9.625" style="7" customWidth="1"/>
     <col min="7943" max="7943" width="9" style="7"/>
     <col min="7944" max="7944" width="9" style="7" bestFit="1" customWidth="1"/>
     <col min="7945" max="8192" width="9" style="7"/>
-    <col min="8193" max="8193" width="11.3984375" style="7" customWidth="1"/>
-    <col min="8194" max="8194" width="9.59765625" style="7" bestFit="1" customWidth="1"/>
+    <col min="8193" max="8193" width="11.375" style="7" customWidth="1"/>
+    <col min="8194" max="8194" width="9.625" style="7" bestFit="1" customWidth="1"/>
     <col min="8195" max="8195" width="9" style="7" bestFit="1" customWidth="1"/>
-    <col min="8196" max="8197" width="8.59765625" style="7" bestFit="1" customWidth="1"/>
-    <col min="8198" max="8198" width="9.59765625" style="7" customWidth="1"/>
+    <col min="8196" max="8197" width="8.625" style="7" bestFit="1" customWidth="1"/>
+    <col min="8198" max="8198" width="9.625" style="7" customWidth="1"/>
     <col min="8199" max="8199" width="9" style="7"/>
     <col min="8200" max="8200" width="9" style="7" bestFit="1" customWidth="1"/>
     <col min="8201" max="8448" width="9" style="7"/>
-    <col min="8449" max="8449" width="11.3984375" style="7" customWidth="1"/>
-    <col min="8450" max="8450" width="9.59765625" style="7" bestFit="1" customWidth="1"/>
+    <col min="8449" max="8449" width="11.375" style="7" customWidth="1"/>
+    <col min="8450" max="8450" width="9.625" style="7" bestFit="1" customWidth="1"/>
     <col min="8451" max="8451" width="9" style="7" bestFit="1" customWidth="1"/>
-    <col min="8452" max="8453" width="8.59765625" style="7" bestFit="1" customWidth="1"/>
-    <col min="8454" max="8454" width="9.59765625" style="7" customWidth="1"/>
+    <col min="8452" max="8453" width="8.625" style="7" bestFit="1" customWidth="1"/>
+    <col min="8454" max="8454" width="9.625" style="7" customWidth="1"/>
     <col min="8455" max="8455" width="9" style="7"/>
     <col min="8456" max="8456" width="9" style="7" bestFit="1" customWidth="1"/>
     <col min="8457" max="8704" width="9" style="7"/>
-    <col min="8705" max="8705" width="11.3984375" style="7" customWidth="1"/>
-    <col min="8706" max="8706" width="9.59765625" style="7" bestFit="1" customWidth="1"/>
+    <col min="8705" max="8705" width="11.375" style="7" customWidth="1"/>
+    <col min="8706" max="8706" width="9.625" style="7" bestFit="1" customWidth="1"/>
     <col min="8707" max="8707" width="9" style="7" bestFit="1" customWidth="1"/>
-    <col min="8708" max="8709" width="8.59765625" style="7" bestFit="1" customWidth="1"/>
-    <col min="8710" max="8710" width="9.59765625" style="7" customWidth="1"/>
+    <col min="8708" max="8709" width="8.625" style="7" bestFit="1" customWidth="1"/>
+    <col min="8710" max="8710" width="9.625" style="7" customWidth="1"/>
     <col min="8711" max="8711" width="9" style="7"/>
     <col min="8712" max="8712" width="9" style="7" bestFit="1" customWidth="1"/>
     <col min="8713" max="8960" width="9" style="7"/>
-    <col min="8961" max="8961" width="11.3984375" style="7" customWidth="1"/>
-    <col min="8962" max="8962" width="9.59765625" style="7" bestFit="1" customWidth="1"/>
+    <col min="8961" max="8961" width="11.375" style="7" customWidth="1"/>
+    <col min="8962" max="8962" width="9.625" style="7" bestFit="1" customWidth="1"/>
     <col min="8963" max="8963" width="9" style="7" bestFit="1" customWidth="1"/>
-    <col min="8964" max="8965" width="8.59765625" style="7" bestFit="1" customWidth="1"/>
-    <col min="8966" max="8966" width="9.59765625" style="7" customWidth="1"/>
+    <col min="8964" max="8965" width="8.625" style="7" bestFit="1" customWidth="1"/>
+    <col min="8966" max="8966" width="9.625" style="7" customWidth="1"/>
     <col min="8967" max="8967" width="9" style="7"/>
     <col min="8968" max="8968" width="9" style="7" bestFit="1" customWidth="1"/>
     <col min="8969" max="9216" width="9" style="7"/>
-    <col min="9217" max="9217" width="11.3984375" style="7" customWidth="1"/>
-    <col min="9218" max="9218" width="9.59765625" style="7" bestFit="1" customWidth="1"/>
+    <col min="9217" max="9217" width="11.375" style="7" customWidth="1"/>
+    <col min="9218" max="9218" width="9.625" style="7" bestFit="1" customWidth="1"/>
     <col min="9219" max="9219" width="9" style="7" bestFit="1" customWidth="1"/>
-    <col min="9220" max="9221" width="8.59765625" style="7" bestFit="1" customWidth="1"/>
-    <col min="9222" max="9222" width="9.59765625" style="7" customWidth="1"/>
+    <col min="9220" max="9221" width="8.625" style="7" bestFit="1" customWidth="1"/>
+    <col min="9222" max="9222" width="9.625" style="7" customWidth="1"/>
     <col min="9223" max="9223" width="9" style="7"/>
     <col min="9224" max="9224" width="9" style="7" bestFit="1" customWidth="1"/>
     <col min="9225" max="9472" width="9" style="7"/>
-    <col min="9473" max="9473" width="11.3984375" style="7" customWidth="1"/>
-    <col min="9474" max="9474" width="9.59765625" style="7" bestFit="1" customWidth="1"/>
+    <col min="9473" max="9473" width="11.375" style="7" customWidth="1"/>
+    <col min="9474" max="9474" width="9.625" style="7" bestFit="1" customWidth="1"/>
     <col min="9475" max="9475" width="9" style="7" bestFit="1" customWidth="1"/>
-    <col min="9476" max="9477" width="8.59765625" style="7" bestFit="1" customWidth="1"/>
-    <col min="9478" max="9478" width="9.59765625" style="7" customWidth="1"/>
+    <col min="9476" max="9477" width="8.625" style="7" bestFit="1" customWidth="1"/>
+    <col min="9478" max="9478" width="9.625" style="7" customWidth="1"/>
     <col min="9479" max="9479" width="9" style="7"/>
     <col min="9480" max="9480" width="9" style="7" bestFit="1" customWidth="1"/>
     <col min="9481" max="9728" width="9" style="7"/>
-    <col min="9729" max="9729" width="11.3984375" style="7" customWidth="1"/>
-    <col min="9730" max="9730" width="9.59765625" style="7" bestFit="1" customWidth="1"/>
+    <col min="9729" max="9729" width="11.375" style="7" customWidth="1"/>
+    <col min="9730" max="9730" width="9.625" style="7" bestFit="1" customWidth="1"/>
     <col min="9731" max="9731" width="9" style="7" bestFit="1" customWidth="1"/>
-    <col min="9732" max="9733" width="8.59765625" style="7" bestFit="1" customWidth="1"/>
-    <col min="9734" max="9734" width="9.59765625" style="7" customWidth="1"/>
+    <col min="9732" max="9733" width="8.625" style="7" bestFit="1" customWidth="1"/>
+    <col min="9734" max="9734" width="9.625" style="7" customWidth="1"/>
     <col min="9735" max="9735" width="9" style="7"/>
     <col min="9736" max="9736" width="9" style="7" bestFit="1" customWidth="1"/>
     <col min="9737" max="9984" width="9" style="7"/>
-    <col min="9985" max="9985" width="11.3984375" style="7" customWidth="1"/>
-    <col min="9986" max="9986" width="9.59765625" style="7" bestFit="1" customWidth="1"/>
+    <col min="9985" max="9985" width="11.375" style="7" customWidth="1"/>
+    <col min="9986" max="9986" width="9.625" style="7" bestFit="1" customWidth="1"/>
     <col min="9987" max="9987" width="9" style="7" bestFit="1" customWidth="1"/>
-    <col min="9988" max="9989" width="8.59765625" style="7" bestFit="1" customWidth="1"/>
-    <col min="9990" max="9990" width="9.59765625" style="7" customWidth="1"/>
+    <col min="9988" max="9989" width="8.625" style="7" bestFit="1" customWidth="1"/>
+    <col min="9990" max="9990" width="9.625" style="7" customWidth="1"/>
     <col min="9991" max="9991" width="9" style="7"/>
     <col min="9992" max="9992" width="9" style="7" bestFit="1" customWidth="1"/>
     <col min="9993" max="10240" width="9" style="7"/>
-    <col min="10241" max="10241" width="11.3984375" style="7" customWidth="1"/>
-    <col min="10242" max="10242" width="9.59765625" style="7" bestFit="1" customWidth="1"/>
+    <col min="10241" max="10241" width="11.375" style="7" customWidth="1"/>
+    <col min="10242" max="10242" width="9.625" style="7" bestFit="1" customWidth="1"/>
     <col min="10243" max="10243" width="9" style="7" bestFit="1" customWidth="1"/>
-    <col min="10244" max="10245" width="8.59765625" style="7" bestFit="1" customWidth="1"/>
-    <col min="10246" max="10246" width="9.59765625" style="7" customWidth="1"/>
+    <col min="10244" max="10245" width="8.625" style="7" bestFit="1" customWidth="1"/>
+    <col min="10246" max="10246" width="9.625" style="7" customWidth="1"/>
     <col min="10247" max="10247" width="9" style="7"/>
     <col min="10248" max="10248" width="9" style="7" bestFit="1" customWidth="1"/>
     <col min="10249" max="10496" width="9" style="7"/>
-    <col min="10497" max="10497" width="11.3984375" style="7" customWidth="1"/>
-    <col min="10498" max="10498" width="9.59765625" style="7" bestFit="1" customWidth="1"/>
+    <col min="10497" max="10497" width="11.375" style="7" customWidth="1"/>
+    <col min="10498" max="10498" width="9.625" style="7" bestFit="1" customWidth="1"/>
     <col min="10499" max="10499" width="9" style="7" bestFit="1" customWidth="1"/>
-    <col min="10500" max="10501" width="8.59765625" style="7" bestFit="1" customWidth="1"/>
-    <col min="10502" max="10502" width="9.59765625" style="7" customWidth="1"/>
+    <col min="10500" max="10501" width="8.625" style="7" bestFit="1" customWidth="1"/>
+    <col min="10502" max="10502" width="9.625" style="7" customWidth="1"/>
     <col min="10503" max="10503" width="9" style="7"/>
     <col min="10504" max="10504" width="9" style="7" bestFit="1" customWidth="1"/>
     <col min="10505" max="10752" width="9" style="7"/>
-    <col min="10753" max="10753" width="11.3984375" style="7" customWidth="1"/>
-    <col min="10754" max="10754" width="9.59765625" style="7" bestFit="1" customWidth="1"/>
+    <col min="10753" max="10753" width="11.375" style="7" customWidth="1"/>
+    <col min="10754" max="10754" width="9.625" style="7" bestFit="1" customWidth="1"/>
     <col min="10755" max="10755" width="9" style="7" bestFit="1" customWidth="1"/>
-    <col min="10756" max="10757" width="8.59765625" style="7" bestFit="1" customWidth="1"/>
-    <col min="10758" max="10758" width="9.59765625" style="7" customWidth="1"/>
+    <col min="10756" max="10757" width="8.625" style="7" bestFit="1" customWidth="1"/>
+    <col min="10758" max="10758" width="9.625" style="7" customWidth="1"/>
     <col min="10759" max="10759" width="9" style="7"/>
     <col min="10760" max="10760" width="9" style="7" bestFit="1" customWidth="1"/>
     <col min="10761" max="11008" width="9" style="7"/>
-    <col min="11009" max="11009" width="11.3984375" style="7" customWidth="1"/>
-    <col min="11010" max="11010" width="9.59765625" style="7" bestFit="1" customWidth="1"/>
+    <col min="11009" max="11009" width="11.375" style="7" customWidth="1"/>
+    <col min="11010" max="11010" width="9.625" style="7" bestFit="1" customWidth="1"/>
     <col min="11011" max="11011" width="9" style="7" bestFit="1" customWidth="1"/>
-    <col min="11012" max="11013" width="8.59765625" style="7" bestFit="1" customWidth="1"/>
-    <col min="11014" max="11014" width="9.59765625" style="7" customWidth="1"/>
+    <col min="11012" max="11013" width="8.625" style="7" bestFit="1" customWidth="1"/>
+    <col min="11014" max="11014" width="9.625" style="7" customWidth="1"/>
     <col min="11015" max="11015" width="9" style="7"/>
     <col min="11016" max="11016" width="9" style="7" bestFit="1" customWidth="1"/>
     <col min="11017" max="11264" width="9" style="7"/>
-    <col min="11265" max="11265" width="11.3984375" style="7" customWidth="1"/>
-    <col min="11266" max="11266" width="9.59765625" style="7" bestFit="1" customWidth="1"/>
+    <col min="11265" max="11265" width="11.375" style="7" customWidth="1"/>
+    <col min="11266" max="11266" width="9.625" style="7" bestFit="1" customWidth="1"/>
     <col min="11267" max="11267" width="9" style="7" bestFit="1" customWidth="1"/>
-    <col min="11268" max="11269" width="8.59765625" style="7" bestFit="1" customWidth="1"/>
-    <col min="11270" max="11270" width="9.59765625" style="7" customWidth="1"/>
+    <col min="11268" max="11269" width="8.625" style="7" bestFit="1" customWidth="1"/>
+    <col min="11270" max="11270" width="9.625" style="7" customWidth="1"/>
     <col min="11271" max="11271" width="9" style="7"/>
     <col min="11272" max="11272" width="9" style="7" bestFit="1" customWidth="1"/>
     <col min="11273" max="11520" width="9" style="7"/>
-    <col min="11521" max="11521" width="11.3984375" style="7" customWidth="1"/>
-    <col min="11522" max="11522" width="9.59765625" style="7" bestFit="1" customWidth="1"/>
+    <col min="11521" max="11521" width="11.375" style="7" customWidth="1"/>
+    <col min="11522" max="11522" width="9.625" style="7" bestFit="1" customWidth="1"/>
     <col min="11523" max="11523" width="9" style="7" bestFit="1" customWidth="1"/>
-    <col min="11524" max="11525" width="8.59765625" style="7" bestFit="1" customWidth="1"/>
-    <col min="11526" max="11526" width="9.59765625" style="7" customWidth="1"/>
+    <col min="11524" max="11525" width="8.625" style="7" bestFit="1" customWidth="1"/>
+    <col min="11526" max="11526" width="9.625" style="7" customWidth="1"/>
     <col min="11527" max="11527" width="9" style="7"/>
     <col min="11528" max="11528" width="9" style="7" bestFit="1" customWidth="1"/>
     <col min="11529" max="11776" width="9" style="7"/>
-    <col min="11777" max="11777" width="11.3984375" style="7" customWidth="1"/>
-    <col min="11778" max="11778" width="9.59765625" style="7" bestFit="1" customWidth="1"/>
+    <col min="11777" max="11777" width="11.375" style="7" customWidth="1"/>
+    <col min="11778" max="11778" width="9.625" style="7" bestFit="1" customWidth="1"/>
     <col min="11779" max="11779" width="9" style="7" bestFit="1" customWidth="1"/>
-    <col min="11780" max="11781" width="8.59765625" style="7" bestFit="1" customWidth="1"/>
-    <col min="11782" max="11782" width="9.59765625" style="7" customWidth="1"/>
+    <col min="11780" max="11781" width="8.625" style="7" bestFit="1" customWidth="1"/>
+    <col min="11782" max="11782" width="9.625" style="7" customWidth="1"/>
     <col min="11783" max="11783" width="9" style="7"/>
     <col min="11784" max="11784" width="9" style="7" bestFit="1" customWidth="1"/>
     <col min="11785" max="12032" width="9" style="7"/>
-    <col min="12033" max="12033" width="11.3984375" style="7" customWidth="1"/>
-    <col min="12034" max="12034" width="9.59765625" style="7" bestFit="1" customWidth="1"/>
+    <col min="12033" max="12033" width="11.375" style="7" customWidth="1"/>
+    <col min="12034" max="12034" width="9.625" style="7" bestFit="1" customWidth="1"/>
     <col min="12035" max="12035" width="9" style="7" bestFit="1" customWidth="1"/>
-    <col min="12036" max="12037" width="8.59765625" style="7" bestFit="1" customWidth="1"/>
-    <col min="12038" max="12038" width="9.59765625" style="7" customWidth="1"/>
+    <col min="12036" max="12037" width="8.625" style="7" bestFit="1" customWidth="1"/>
+    <col min="12038" max="12038" width="9.625" style="7" customWidth="1"/>
     <col min="12039" max="12039" width="9" style="7"/>
     <col min="12040" max="12040" width="9" style="7" bestFit="1" customWidth="1"/>
     <col min="12041" max="12288" width="9" style="7"/>
-    <col min="12289" max="12289" width="11.3984375" style="7" customWidth="1"/>
-    <col min="12290" max="12290" width="9.59765625" style="7" bestFit="1" customWidth="1"/>
+    <col min="12289" max="12289" width="11.375" style="7" customWidth="1"/>
+    <col min="12290" max="12290" width="9.625" style="7" bestFit="1" customWidth="1"/>
     <col min="12291" max="12291" width="9" style="7" bestFit="1" customWidth="1"/>
-    <col min="12292" max="12293" width="8.59765625" style="7" bestFit="1" customWidth="1"/>
-    <col min="12294" max="12294" width="9.59765625" style="7" customWidth="1"/>
+    <col min="12292" max="12293" width="8.625" style="7" bestFit="1" customWidth="1"/>
+    <col min="12294" max="12294" width="9.625" style="7" customWidth="1"/>
     <col min="12295" max="12295" width="9" style="7"/>
     <col min="12296" max="12296" width="9" style="7" bestFit="1" customWidth="1"/>
     <col min="12297" max="12544" width="9" style="7"/>
-    <col min="12545" max="12545" width="11.3984375" style="7" customWidth="1"/>
-    <col min="12546" max="12546" width="9.59765625" style="7" bestFit="1" customWidth="1"/>
+    <col min="12545" max="12545" width="11.375" style="7" customWidth="1"/>
+    <col min="12546" max="12546" width="9.625" style="7" bestFit="1" customWidth="1"/>
     <col min="12547" max="12547" width="9" style="7" bestFit="1" customWidth="1"/>
-    <col min="12548" max="12549" width="8.59765625" style="7" bestFit="1" customWidth="1"/>
-    <col min="12550" max="12550" width="9.59765625" style="7" customWidth="1"/>
+    <col min="12548" max="12549" width="8.625" style="7" bestFit="1" customWidth="1"/>
+    <col min="12550" max="12550" width="9.625" style="7" customWidth="1"/>
     <col min="12551" max="12551" width="9" style="7"/>
     <col min="12552" max="12552" width="9" style="7" bestFit="1" customWidth="1"/>
     <col min="12553" max="12800" width="9" style="7"/>
-    <col min="12801" max="12801" width="11.3984375" style="7" customWidth="1"/>
-    <col min="12802" max="12802" width="9.59765625" style="7" bestFit="1" customWidth="1"/>
+    <col min="12801" max="12801" width="11.375" style="7" customWidth="1"/>
+    <col min="12802" max="12802" width="9.625" style="7" bestFit="1" customWidth="1"/>
     <col min="12803" max="12803" width="9" style="7" bestFit="1" customWidth="1"/>
-    <col min="12804" max="12805" width="8.59765625" style="7" bestFit="1" customWidth="1"/>
-    <col min="12806" max="12806" width="9.59765625" style="7" customWidth="1"/>
+    <col min="12804" max="12805" width="8.625" style="7" bestFit="1" customWidth="1"/>
+    <col min="12806" max="12806" width="9.625" style="7" customWidth="1"/>
     <col min="12807" max="12807" width="9" style="7"/>
     <col min="12808" max="12808" width="9" style="7" bestFit="1" customWidth="1"/>
     <col min="12809" max="13056" width="9" style="7"/>
-    <col min="13057" max="13057" width="11.3984375" style="7" customWidth="1"/>
-    <col min="13058" max="13058" width="9.59765625" style="7" bestFit="1" customWidth="1"/>
+    <col min="13057" max="13057" width="11.375" style="7" customWidth="1"/>
+    <col min="13058" max="13058" width="9.625" style="7" bestFit="1" customWidth="1"/>
     <col min="13059" max="13059" width="9" style="7" bestFit="1" customWidth="1"/>
-    <col min="13060" max="13061" width="8.59765625" style="7" bestFit="1" customWidth="1"/>
-    <col min="13062" max="13062" width="9.59765625" style="7" customWidth="1"/>
+    <col min="13060" max="13061" width="8.625" style="7" bestFit="1" customWidth="1"/>
+    <col min="13062" max="13062" width="9.625" style="7" customWidth="1"/>
     <col min="13063" max="13063" width="9" style="7"/>
     <col min="13064" max="13064" width="9" style="7" bestFit="1" customWidth="1"/>
     <col min="13065" max="13312" width="9" style="7"/>
-    <col min="13313" max="13313" width="11.3984375" style="7" customWidth="1"/>
-    <col min="13314" max="13314" width="9.59765625" style="7" bestFit="1" customWidth="1"/>
+    <col min="13313" max="13313" width="11.375" style="7" customWidth="1"/>
+    <col min="13314" max="13314" width="9.625" style="7" bestFit="1" customWidth="1"/>
     <col min="13315" max="13315" width="9" style="7" bestFit="1" customWidth="1"/>
-    <col min="13316" max="13317" width="8.59765625" style="7" bestFit="1" customWidth="1"/>
-    <col min="13318" max="13318" width="9.59765625" style="7" customWidth="1"/>
+    <col min="13316" max="13317" width="8.625" style="7" bestFit="1" customWidth="1"/>
+    <col min="13318" max="13318" width="9.625" style="7" customWidth="1"/>
     <col min="13319" max="13319" width="9" style="7"/>
     <col min="13320" max="13320" width="9" style="7" bestFit="1" customWidth="1"/>
     <col min="13321" max="13568" width="9" style="7"/>
-    <col min="13569" max="13569" width="11.3984375" style="7" customWidth="1"/>
-    <col min="13570" max="13570" width="9.59765625" style="7" bestFit="1" customWidth="1"/>
+    <col min="13569" max="13569" width="11.375" style="7" customWidth="1"/>
+    <col min="13570" max="13570" width="9.625" style="7" bestFit="1" customWidth="1"/>
     <col min="13571" max="13571" width="9" style="7" bestFit="1" customWidth="1"/>
-    <col min="13572" max="13573" width="8.59765625" style="7" bestFit="1" customWidth="1"/>
-    <col min="13574" max="13574" width="9.59765625" style="7" customWidth="1"/>
+    <col min="13572" max="13573" width="8.625" style="7" bestFit="1" customWidth="1"/>
+    <col min="13574" max="13574" width="9.625" style="7" customWidth="1"/>
     <col min="13575" max="13575" width="9" style="7"/>
     <col min="13576" max="13576" width="9" style="7" bestFit="1" customWidth="1"/>
     <col min="13577" max="13824" width="9" style="7"/>
-    <col min="13825" max="13825" width="11.3984375" style="7" customWidth="1"/>
-    <col min="13826" max="13826" width="9.59765625" style="7" bestFit="1" customWidth="1"/>
+    <col min="13825" max="13825" width="11.375" style="7" customWidth="1"/>
+    <col min="13826" max="13826" width="9.625" style="7" bestFit="1" customWidth="1"/>
     <col min="13827" max="13827" width="9" style="7" bestFit="1" customWidth="1"/>
-    <col min="13828" max="13829" width="8.59765625" style="7" bestFit="1" customWidth="1"/>
-    <col min="13830" max="13830" width="9.59765625" style="7" customWidth="1"/>
+    <col min="13828" max="13829" width="8.625" style="7" bestFit="1" customWidth="1"/>
+    <col min="13830" max="13830" width="9.625" style="7" customWidth="1"/>
     <col min="13831" max="13831" width="9" style="7"/>
     <col min="13832" max="13832" width="9" style="7" bestFit="1" customWidth="1"/>
     <col min="13833" max="14080" width="9" style="7"/>
-    <col min="14081" max="14081" width="11.3984375" style="7" customWidth="1"/>
-    <col min="14082" max="14082" width="9.59765625" style="7" bestFit="1" customWidth="1"/>
+    <col min="14081" max="14081" width="11.375" style="7" customWidth="1"/>
+    <col min="14082" max="14082" width="9.625" style="7" bestFit="1" customWidth="1"/>
     <col min="14083" max="14083" width="9" style="7" bestFit="1" customWidth="1"/>
-    <col min="14084" max="14085" width="8.59765625" style="7" bestFit="1" customWidth="1"/>
-    <col min="14086" max="14086" width="9.59765625" style="7" customWidth="1"/>
+    <col min="14084" max="14085" width="8.625" style="7" bestFit="1" customWidth="1"/>
+    <col min="14086" max="14086" width="9.625" style="7" customWidth="1"/>
     <col min="14087" max="14087" width="9" style="7"/>
     <col min="14088" max="14088" width="9" style="7" bestFit="1" customWidth="1"/>
     <col min="14089" max="14336" width="9" style="7"/>
-    <col min="14337" max="14337" width="11.3984375" style="7" customWidth="1"/>
-    <col min="14338" max="14338" width="9.59765625" style="7" bestFit="1" customWidth="1"/>
+    <col min="14337" max="14337" width="11.375" style="7" customWidth="1"/>
+    <col min="14338" max="14338" width="9.625" style="7" bestFit="1" customWidth="1"/>
     <col min="14339" max="14339" width="9" style="7" bestFit="1" customWidth="1"/>
-    <col min="14340" max="14341" width="8.59765625" style="7" bestFit="1" customWidth="1"/>
-    <col min="14342" max="14342" width="9.59765625" style="7" customWidth="1"/>
+    <col min="14340" max="14341" width="8.625" style="7" bestFit="1" customWidth="1"/>
+    <col min="14342" max="14342" width="9.625" style="7" customWidth="1"/>
     <col min="14343" max="14343" width="9" style="7"/>
     <col min="14344" max="14344" width="9" style="7" bestFit="1" customWidth="1"/>
     <col min="14345" max="14592" width="9" style="7"/>
-    <col min="14593" max="14593" width="11.3984375" style="7" customWidth="1"/>
-    <col min="14594" max="14594" width="9.59765625" style="7" bestFit="1" customWidth="1"/>
+    <col min="14593" max="14593" width="11.375" style="7" customWidth="1"/>
+    <col min="14594" max="14594" width="9.625" style="7" bestFit="1" customWidth="1"/>
     <col min="14595" max="14595" width="9" style="7" bestFit="1" customWidth="1"/>
-    <col min="14596" max="14597" width="8.59765625" style="7" bestFit="1" customWidth="1"/>
-    <col min="14598" max="14598" width="9.59765625" style="7" customWidth="1"/>
+    <col min="14596" max="14597" width="8.625" style="7" bestFit="1" customWidth="1"/>
+    <col min="14598" max="14598" width="9.625" style="7" customWidth="1"/>
     <col min="14599" max="14599" width="9" style="7"/>
     <col min="14600" max="14600" width="9" style="7" bestFit="1" customWidth="1"/>
     <col min="14601" max="14848" width="9" style="7"/>
-    <col min="14849" max="14849" width="11.3984375" style="7" customWidth="1"/>
-    <col min="14850" max="14850" width="9.59765625" style="7" bestFit="1" customWidth="1"/>
+    <col min="14849" max="14849" width="11.375" style="7" customWidth="1"/>
+    <col min="14850" max="14850" width="9.625" style="7" bestFit="1" customWidth="1"/>
     <col min="14851" max="14851" width="9" style="7" bestFit="1" customWidth="1"/>
-    <col min="14852" max="14853" width="8.59765625" style="7" bestFit="1" customWidth="1"/>
-    <col min="14854" max="14854" width="9.59765625" style="7" customWidth="1"/>
+    <col min="14852" max="14853" width="8.625" style="7" bestFit="1" customWidth="1"/>
+    <col min="14854" max="14854" width="9.625" style="7" customWidth="1"/>
     <col min="14855" max="14855" width="9" style="7"/>
     <col min="14856" max="14856" width="9" style="7" bestFit="1" customWidth="1"/>
     <col min="14857" max="15104" width="9" style="7"/>
-    <col min="15105" max="15105" width="11.3984375" style="7" customWidth="1"/>
-    <col min="15106" max="15106" width="9.59765625" style="7" bestFit="1" customWidth="1"/>
+    <col min="15105" max="15105" width="11.375" style="7" customWidth="1"/>
+    <col min="15106" max="15106" width="9.625" style="7" bestFit="1" customWidth="1"/>
     <col min="15107" max="15107" width="9" style="7" bestFit="1" customWidth="1"/>
-    <col min="15108" max="15109" width="8.59765625" style="7" bestFit="1" customWidth="1"/>
-    <col min="15110" max="15110" width="9.59765625" style="7" customWidth="1"/>
+    <col min="15108" max="15109" width="8.625" style="7" bestFit="1" customWidth="1"/>
+    <col min="15110" max="15110" width="9.625" style="7" customWidth="1"/>
     <col min="15111" max="15111" width="9" style="7"/>
     <col min="15112" max="15112" width="9" style="7" bestFit="1" customWidth="1"/>
     <col min="15113" max="15360" width="9" style="7"/>
-    <col min="15361" max="15361" width="11.3984375" style="7" customWidth="1"/>
-    <col min="15362" max="15362" width="9.59765625" style="7" bestFit="1" customWidth="1"/>
+    <col min="15361" max="15361" width="11.375" style="7" customWidth="1"/>
+    <col min="15362" max="15362" width="9.625" style="7" bestFit="1" customWidth="1"/>
     <col min="15363" max="15363" width="9" style="7" bestFit="1" customWidth="1"/>
-    <col min="15364" max="15365" width="8.59765625" style="7" bestFit="1" customWidth="1"/>
-    <col min="15366" max="15366" width="9.59765625" style="7" customWidth="1"/>
+    <col min="15364" max="15365" width="8.625" style="7" bestFit="1" customWidth="1"/>
+    <col min="15366" max="15366" width="9.625" style="7" customWidth="1"/>
     <col min="15367" max="15367" width="9" style="7"/>
     <col min="15368" max="15368" width="9" style="7" bestFit="1" customWidth="1"/>
     <col min="15369" max="15616" width="9" style="7"/>
-    <col min="15617" max="15617" width="11.3984375" style="7" customWidth="1"/>
-    <col min="15618" max="15618" width="9.59765625" style="7" bestFit="1" customWidth="1"/>
+    <col min="15617" max="15617" width="11.375" style="7" customWidth="1"/>
+    <col min="15618" max="15618" width="9.625" style="7" bestFit="1" customWidth="1"/>
     <col min="15619" max="15619" width="9" style="7" bestFit="1" customWidth="1"/>
-    <col min="15620" max="15621" width="8.59765625" style="7" bestFit="1" customWidth="1"/>
-    <col min="15622" max="15622" width="9.59765625" style="7" customWidth="1"/>
+    <col min="15620" max="15621" width="8.625" style="7" bestFit="1" customWidth="1"/>
+    <col min="15622" max="15622" width="9.625" style="7" customWidth="1"/>
     <col min="15623" max="15623" width="9" style="7"/>
     <col min="15624" max="15624" width="9" style="7" bestFit="1" customWidth="1"/>
     <col min="15625" max="15872" width="9" style="7"/>
-    <col min="15873" max="15873" width="11.3984375" style="7" customWidth="1"/>
-    <col min="15874" max="15874" width="9.59765625" style="7" bestFit="1" customWidth="1"/>
+    <col min="15873" max="15873" width="11.375" style="7" customWidth="1"/>
+    <col min="15874" max="15874" width="9.625" style="7" bestFit="1" customWidth="1"/>
     <col min="15875" max="15875" width="9" style="7" bestFit="1" customWidth="1"/>
-    <col min="15876" max="15877" width="8.59765625" style="7" bestFit="1" customWidth="1"/>
-    <col min="15878" max="15878" width="9.59765625" style="7" customWidth="1"/>
+    <col min="15876" max="15877" width="8.625" style="7" bestFit="1" customWidth="1"/>
+    <col min="15878" max="15878" width="9.625" style="7" customWidth="1"/>
     <col min="15879" max="15879" width="9" style="7"/>
     <col min="15880" max="15880" width="9" style="7" bestFit="1" customWidth="1"/>
     <col min="15881" max="16128" width="9" style="7"/>
-    <col min="16129" max="16129" width="11.3984375" style="7" customWidth="1"/>
-    <col min="16130" max="16130" width="9.59765625" style="7" bestFit="1" customWidth="1"/>
+    <col min="16129" max="16129" width="11.375" style="7" customWidth="1"/>
+    <col min="16130" max="16130" width="9.625" style="7" bestFit="1" customWidth="1"/>
     <col min="16131" max="16131" width="9" style="7" bestFit="1" customWidth="1"/>
-    <col min="16132" max="16133" width="8.59765625" style="7" bestFit="1" customWidth="1"/>
-    <col min="16134" max="16134" width="9.59765625" style="7" customWidth="1"/>
+    <col min="16132" max="16133" width="8.625" style="7" bestFit="1" customWidth="1"/>
+    <col min="16134" max="16134" width="9.625" style="7" customWidth="1"/>
     <col min="16135" max="16135" width="9" style="7"/>
     <col min="16136" max="16136" width="9" style="7" bestFit="1" customWidth="1"/>
     <col min="16137" max="16384" width="9" style="7"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" ht="66" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:8" ht="65.650000000000006" x14ac:dyDescent="0.4">
       <c r="A1" s="1" t="s">
         <v>11</v>
       </c>
@@ -7994,7 +7945,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="2" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:8" hidden="1" x14ac:dyDescent="0.4">
       <c r="A2" s="4">
         <v>44338</v>
       </c>
@@ -8008,7 +7959,7 @@
       </c>
       <c r="H2" s="5"/>
     </row>
-    <row r="3" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:8" hidden="1" x14ac:dyDescent="0.4">
       <c r="A3" s="4">
         <v>44339</v>
       </c>
@@ -8022,7 +7973,7 @@
       </c>
       <c r="H3" s="5"/>
     </row>
-    <row r="4" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:8" hidden="1" x14ac:dyDescent="0.4">
       <c r="A4" s="4">
         <v>44340</v>
       </c>
@@ -8036,7 +7987,7 @@
       </c>
       <c r="H4" s="5"/>
     </row>
-    <row r="5" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:8" hidden="1" x14ac:dyDescent="0.4">
       <c r="A5" s="4">
         <v>44341</v>
       </c>
@@ -8050,7 +8001,7 @@
       </c>
       <c r="H5" s="5"/>
     </row>
-    <row r="6" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:8" hidden="1" x14ac:dyDescent="0.4">
       <c r="A6" s="4">
         <v>44342</v>
       </c>
@@ -8064,7 +8015,7 @@
       </c>
       <c r="H6" s="5"/>
     </row>
-    <row r="7" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:8" hidden="1" x14ac:dyDescent="0.4">
       <c r="A7" s="4">
         <v>44343</v>
       </c>
@@ -8078,7 +8029,7 @@
       </c>
       <c r="H7" s="5"/>
     </row>
-    <row r="8" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:8" x14ac:dyDescent="0.4">
       <c r="A8" s="4">
         <v>44344</v>
       </c>
@@ -8102,7 +8053,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="9" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:8" x14ac:dyDescent="0.4">
       <c r="A9" s="4">
         <v>44345</v>
       </c>
@@ -8126,7 +8077,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="10" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:8" x14ac:dyDescent="0.4">
       <c r="A10" s="4">
         <v>44346</v>
       </c>
@@ -8150,7 +8101,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="11" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:8" x14ac:dyDescent="0.4">
       <c r="A11" s="4">
         <v>44347</v>
       </c>
@@ -8174,7 +8125,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="12" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:8" x14ac:dyDescent="0.4">
       <c r="A12" s="4">
         <v>44348</v>
       </c>
@@ -8198,7 +8149,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="13" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:8" x14ac:dyDescent="0.4">
       <c r="A13" s="4">
         <v>44349</v>
       </c>
@@ -8222,7 +8173,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="14" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:8" x14ac:dyDescent="0.4">
       <c r="A14" s="4">
         <v>44350</v>
       </c>
@@ -8246,7 +8197,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="15" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:8" x14ac:dyDescent="0.4">
       <c r="A15" s="4">
         <v>44351</v>
       </c>
@@ -8270,7 +8221,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="16" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:8" x14ac:dyDescent="0.4">
       <c r="A16" s="4">
         <v>44352</v>
       </c>
@@ -8294,7 +8245,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="17" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:8" x14ac:dyDescent="0.4">
       <c r="A17" s="4">
         <v>44353</v>
       </c>
@@ -8318,7 +8269,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="18" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:8" x14ac:dyDescent="0.4">
       <c r="A18" s="4">
         <v>44354</v>
       </c>
@@ -8342,7 +8293,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="19" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:8" x14ac:dyDescent="0.4">
       <c r="A19" s="4">
         <v>44355</v>
       </c>
@@ -8366,7 +8317,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="20" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:8" x14ac:dyDescent="0.4">
       <c r="A20" s="4">
         <v>44356</v>
       </c>
@@ -8390,7 +8341,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="21" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:8" x14ac:dyDescent="0.4">
       <c r="A21" s="4">
         <v>44357</v>
       </c>
@@ -8414,7 +8365,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="22" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:8" x14ac:dyDescent="0.4">
       <c r="A22" s="4">
         <v>44358</v>
       </c>
@@ -8438,7 +8389,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="23" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:8" x14ac:dyDescent="0.4">
       <c r="A23" s="4">
         <v>44359</v>
       </c>
@@ -8462,7 +8413,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="24" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:8" x14ac:dyDescent="0.4">
       <c r="A24" s="4">
         <v>44360</v>
       </c>
@@ -8486,7 +8437,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="25" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:8" x14ac:dyDescent="0.4">
       <c r="A25" s="4">
         <v>44361</v>
       </c>
@@ -8510,7 +8461,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="26" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:8" x14ac:dyDescent="0.4">
       <c r="A26" s="4">
         <v>44362</v>
       </c>
@@ -8534,7 +8485,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="27" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:8" x14ac:dyDescent="0.4">
       <c r="A27" s="4">
         <v>44363</v>
       </c>
@@ -8558,7 +8509,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="28" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:8" x14ac:dyDescent="0.4">
       <c r="A28" s="4">
         <v>44364</v>
       </c>
@@ -8582,7 +8533,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="29" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:8" x14ac:dyDescent="0.4">
       <c r="A29" s="4">
         <v>44365</v>
       </c>
@@ -8606,7 +8557,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="30" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:8" x14ac:dyDescent="0.4">
       <c r="A30" s="4">
         <v>44366</v>
       </c>
@@ -8630,7 +8581,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="31" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:8" x14ac:dyDescent="0.4">
       <c r="A31" s="4">
         <v>44367</v>
       </c>
@@ -8654,7 +8605,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="32" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:8" x14ac:dyDescent="0.4">
       <c r="A32" s="4">
         <v>44368</v>
       </c>
@@ -8678,7 +8629,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="33" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:8" x14ac:dyDescent="0.4">
       <c r="A33" s="4">
         <v>44369</v>
       </c>
@@ -8702,7 +8653,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="34" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:8" x14ac:dyDescent="0.4">
       <c r="A34" s="4">
         <v>44370</v>
       </c>
@@ -8726,7 +8677,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="35" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:8" x14ac:dyDescent="0.4">
       <c r="A35" s="4">
         <v>44371</v>
       </c>
@@ -8750,7 +8701,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="36" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:8" x14ac:dyDescent="0.4">
       <c r="A36" s="4">
         <v>44372</v>
       </c>
@@ -8774,7 +8725,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="37" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:8" x14ac:dyDescent="0.4">
       <c r="A37" s="4">
         <v>44373</v>
       </c>
@@ -8798,7 +8749,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="38" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:8" x14ac:dyDescent="0.4">
       <c r="A38" s="4">
         <v>44374</v>
       </c>
@@ -8822,7 +8773,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="39" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:8" x14ac:dyDescent="0.4">
       <c r="A39" s="4">
         <v>44375</v>
       </c>
@@ -8846,7 +8797,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="40" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:8" x14ac:dyDescent="0.4">
       <c r="A40" s="4">
         <v>44376</v>
       </c>
@@ -8870,7 +8821,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="41" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:8" x14ac:dyDescent="0.4">
       <c r="A41" s="4">
         <v>44377</v>
       </c>
@@ -8894,7 +8845,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="42" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:8" x14ac:dyDescent="0.4">
       <c r="A42" s="4">
         <v>44378</v>
       </c>
@@ -8918,7 +8869,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="43" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="43" spans="1:8" x14ac:dyDescent="0.4">
       <c r="A43" s="4">
         <v>44379</v>
       </c>
@@ -8942,7 +8893,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="44" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="44" spans="1:8" x14ac:dyDescent="0.4">
       <c r="A44" s="4">
         <v>44380</v>
       </c>
@@ -8966,7 +8917,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="45" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="45" spans="1:8" x14ac:dyDescent="0.4">
       <c r="A45" s="4">
         <v>44381</v>
       </c>
@@ -8990,7 +8941,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="46" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="46" spans="1:8" x14ac:dyDescent="0.4">
       <c r="A46" s="4">
         <v>44382</v>
       </c>
@@ -9014,7 +8965,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="47" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="47" spans="1:8" x14ac:dyDescent="0.4">
       <c r="A47" s="4">
         <v>44383</v>
       </c>
@@ -9038,7 +8989,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="48" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="48" spans="1:8" x14ac:dyDescent="0.4">
       <c r="A48" s="4">
         <v>44384</v>
       </c>
@@ -9062,7 +9013,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="49" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="49" spans="1:8" x14ac:dyDescent="0.4">
       <c r="A49" s="4">
         <v>44385</v>
       </c>
@@ -9086,7 +9037,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="50" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="50" spans="1:8" x14ac:dyDescent="0.4">
       <c r="A50" s="4">
         <v>44386</v>
       </c>
@@ -9110,7 +9061,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="51" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="51" spans="1:8" x14ac:dyDescent="0.4">
       <c r="A51" s="4">
         <v>44387</v>
       </c>
@@ -9134,7 +9085,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="52" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="52" spans="1:8" x14ac:dyDescent="0.4">
       <c r="A52" s="4">
         <v>44388</v>
       </c>
@@ -9158,7 +9109,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="53" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="53" spans="1:8" x14ac:dyDescent="0.4">
       <c r="A53" s="4">
         <v>44389</v>
       </c>
@@ -9182,7 +9133,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="54" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="54" spans="1:8" x14ac:dyDescent="0.4">
       <c r="A54" s="4">
         <v>44390</v>
       </c>
@@ -9206,7 +9157,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="55" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="55" spans="1:8" x14ac:dyDescent="0.4">
       <c r="A55" s="4">
         <v>44391</v>
       </c>
@@ -9230,7 +9181,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="56" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="56" spans="1:8" x14ac:dyDescent="0.4">
       <c r="A56" s="4">
         <v>44392</v>
       </c>
@@ -9254,7 +9205,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="57" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="57" spans="1:8" x14ac:dyDescent="0.4">
       <c r="A57" s="4">
         <v>44393</v>
       </c>
@@ -9278,7 +9229,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="58" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="58" spans="1:8" x14ac:dyDescent="0.4">
       <c r="A58" s="4">
         <v>44394</v>
       </c>
@@ -9302,7 +9253,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="59" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="59" spans="1:8" x14ac:dyDescent="0.4">
       <c r="A59" s="4">
         <v>44395</v>
       </c>
@@ -9326,7 +9277,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="60" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="60" spans="1:8" x14ac:dyDescent="0.4">
       <c r="A60" s="4">
         <v>44396</v>
       </c>
@@ -9350,7 +9301,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="61" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="61" spans="1:8" x14ac:dyDescent="0.4">
       <c r="A61" s="4">
         <v>44397</v>
       </c>
@@ -9374,7 +9325,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="62" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="62" spans="1:8" x14ac:dyDescent="0.4">
       <c r="A62" s="4">
         <v>44398</v>
       </c>
@@ -9398,7 +9349,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="63" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="63" spans="1:8" x14ac:dyDescent="0.4">
       <c r="A63" s="4">
         <v>44399</v>
       </c>
@@ -9422,7 +9373,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="64" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="64" spans="1:8" x14ac:dyDescent="0.4">
       <c r="A64" s="4">
         <v>44400</v>
       </c>
@@ -9446,7 +9397,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="65" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="65" spans="1:8" x14ac:dyDescent="0.4">
       <c r="A65" s="4">
         <v>44401</v>
       </c>
@@ -9470,7 +9421,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="66" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="66" spans="1:8" x14ac:dyDescent="0.4">
       <c r="A66" s="4">
         <v>44402</v>
       </c>
@@ -9494,7 +9445,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="67" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="67" spans="1:8" x14ac:dyDescent="0.4">
       <c r="A67" s="4">
         <v>44403</v>
       </c>
@@ -9518,7 +9469,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="68" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="68" spans="1:8" x14ac:dyDescent="0.4">
       <c r="A68" s="4">
         <v>44404</v>
       </c>
@@ -9542,7 +9493,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="69" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="69" spans="1:8" x14ac:dyDescent="0.4">
       <c r="A69" s="4">
         <v>44405</v>
       </c>
@@ -9566,7 +9517,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="70" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="70" spans="1:8" x14ac:dyDescent="0.4">
       <c r="A70" s="4">
         <v>44406</v>
       </c>
@@ -9590,7 +9541,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="71" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="71" spans="1:8" x14ac:dyDescent="0.4">
       <c r="A71" s="4">
         <v>44407</v>
       </c>
@@ -9614,7 +9565,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="72" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="72" spans="1:8" x14ac:dyDescent="0.4">
       <c r="A72" s="4">
         <v>44408</v>
       </c>
@@ -9638,7 +9589,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="73" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="73" spans="1:8" x14ac:dyDescent="0.4">
       <c r="A73" s="4">
         <v>44409</v>
       </c>
@@ -9662,7 +9613,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="74" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="74" spans="1:8" x14ac:dyDescent="0.4">
       <c r="A74" s="4">
         <v>44410</v>
       </c>
@@ -9686,7 +9637,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="75" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="75" spans="1:8" x14ac:dyDescent="0.4">
       <c r="A75" s="4">
         <v>44411</v>
       </c>
@@ -9710,7 +9661,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="76" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="76" spans="1:8" x14ac:dyDescent="0.4">
       <c r="A76" s="4">
         <v>44412</v>
       </c>
@@ -9734,7 +9685,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="77" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="77" spans="1:8" x14ac:dyDescent="0.4">
       <c r="A77" s="4">
         <v>44413</v>
       </c>
@@ -9758,7 +9709,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="78" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="78" spans="1:8" x14ac:dyDescent="0.4">
       <c r="A78" s="4">
         <v>44414</v>
       </c>
@@ -9782,7 +9733,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="79" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="79" spans="1:8" x14ac:dyDescent="0.4">
       <c r="A79" s="4">
         <v>44415</v>
       </c>
@@ -9806,7 +9757,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="80" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="80" spans="1:8" x14ac:dyDescent="0.4">
       <c r="A80" s="4">
         <v>44416</v>
       </c>
@@ -9830,7 +9781,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="81" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="81" spans="1:8" x14ac:dyDescent="0.4">
       <c r="A81" s="4">
         <v>44417</v>
       </c>
@@ -9854,7 +9805,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="82" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="82" spans="1:8" x14ac:dyDescent="0.4">
       <c r="A82" s="4">
         <v>44418</v>
       </c>
@@ -9878,7 +9829,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="83" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="83" spans="1:8" x14ac:dyDescent="0.4">
       <c r="A83" s="4">
         <v>44419</v>
       </c>
@@ -9902,7 +9853,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="84" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="84" spans="1:8" x14ac:dyDescent="0.4">
       <c r="A84" s="4">
         <v>44420</v>
       </c>
@@ -9926,7 +9877,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="85" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="85" spans="1:8" x14ac:dyDescent="0.4">
       <c r="A85" s="4">
         <v>44421</v>
       </c>
@@ -9950,7 +9901,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="86" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="86" spans="1:8" x14ac:dyDescent="0.4">
       <c r="A86" s="4">
         <v>44422</v>
       </c>
@@ -9974,7 +9925,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="87" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="87" spans="1:8" x14ac:dyDescent="0.4">
       <c r="A87" s="4">
         <v>44423</v>
       </c>
@@ -9998,7 +9949,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="88" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="88" spans="1:8" x14ac:dyDescent="0.4">
       <c r="A88" s="4">
         <v>44424</v>
       </c>
@@ -10022,7 +9973,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="89" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="89" spans="1:8" x14ac:dyDescent="0.4">
       <c r="A89" s="4">
         <v>44425</v>
       </c>
@@ -10046,7 +9997,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="90" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="90" spans="1:8" x14ac:dyDescent="0.4">
       <c r="A90" s="4">
         <v>44426</v>
       </c>
@@ -10070,7 +10021,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="91" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="91" spans="1:8" x14ac:dyDescent="0.4">
       <c r="A91" s="4">
         <v>44427</v>
       </c>
@@ -10094,7 +10045,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="92" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="92" spans="1:8" x14ac:dyDescent="0.4">
       <c r="A92" s="4">
         <v>44428</v>
       </c>
@@ -10118,7 +10069,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="93" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="93" spans="1:8" x14ac:dyDescent="0.4">
       <c r="A93" s="4">
         <v>44429</v>
       </c>
@@ -10142,7 +10093,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="94" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="94" spans="1:8" x14ac:dyDescent="0.4">
       <c r="A94" s="4">
         <v>44430</v>
       </c>
@@ -10166,7 +10117,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="95" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="95" spans="1:8" x14ac:dyDescent="0.4">
       <c r="A95" s="4">
         <v>44431</v>
       </c>
@@ -10190,7 +10141,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="96" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="96" spans="1:8" x14ac:dyDescent="0.4">
       <c r="A96" s="4">
         <v>44432</v>
       </c>
@@ -10214,7 +10165,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="97" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="97" spans="1:8" x14ac:dyDescent="0.4">
       <c r="A97" s="4">
         <v>44433</v>
       </c>
@@ -10238,7 +10189,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="98" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="98" spans="1:8" x14ac:dyDescent="0.4">
       <c r="A98" s="4">
         <v>44434</v>
       </c>
@@ -10262,7 +10213,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="99" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="99" spans="1:8" x14ac:dyDescent="0.4">
       <c r="A99" s="4">
         <v>44435</v>
       </c>
@@ -10286,7 +10237,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="100" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="100" spans="1:8" x14ac:dyDescent="0.4">
       <c r="A100" s="4">
         <v>44436</v>
       </c>
@@ -10310,7 +10261,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="101" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="101" spans="1:8" x14ac:dyDescent="0.4">
       <c r="A101" s="4">
         <v>44437</v>
       </c>
@@ -10334,7 +10285,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="102" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="102" spans="1:8" x14ac:dyDescent="0.4">
       <c r="A102" s="4">
         <v>44438</v>
       </c>
@@ -10358,7 +10309,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="103" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="103" spans="1:8" x14ac:dyDescent="0.4">
       <c r="A103" s="4">
         <v>44439</v>
       </c>
@@ -10382,7 +10333,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="104" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="104" spans="1:8" x14ac:dyDescent="0.4">
       <c r="A104" s="4">
         <v>44440</v>
       </c>
@@ -10406,7 +10357,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="105" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="105" spans="1:8" x14ac:dyDescent="0.4">
       <c r="A105" s="4">
         <v>44441</v>
       </c>
@@ -10430,7 +10381,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="106" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="106" spans="1:8" x14ac:dyDescent="0.4">
       <c r="A106" s="4">
         <v>44442</v>
       </c>
@@ -10454,7 +10405,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="107" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="107" spans="1:8" x14ac:dyDescent="0.4">
       <c r="A107" s="4">
         <v>44443</v>
       </c>
@@ -10478,7 +10429,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="108" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="108" spans="1:8" x14ac:dyDescent="0.4">
       <c r="A108" s="4">
         <v>44444</v>
       </c>
@@ -10502,7 +10453,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="109" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="109" spans="1:8" x14ac:dyDescent="0.4">
       <c r="A109" s="4">
         <v>44445</v>
       </c>
@@ -10526,7 +10477,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="110" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="110" spans="1:8" x14ac:dyDescent="0.4">
       <c r="A110" s="4">
         <v>44446</v>
       </c>
@@ -10550,7 +10501,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="111" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="111" spans="1:8" x14ac:dyDescent="0.4">
       <c r="A111" s="4">
         <v>44447</v>
       </c>
@@ -10574,7 +10525,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="112" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="112" spans="1:8" x14ac:dyDescent="0.4">
       <c r="A112" s="4">
         <v>44448</v>
       </c>
@@ -10598,7 +10549,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="113" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="113" spans="1:8" x14ac:dyDescent="0.4">
       <c r="A113" s="4">
         <v>44449</v>
       </c>
@@ -10622,7 +10573,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="114" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="114" spans="1:8" x14ac:dyDescent="0.4">
       <c r="A114" s="8" t="s">
         <v>5</v>
       </c>

</xml_diff>